<commit_message>
Correzioni mancato accreditamento issue #220
Mancato accreditamento A1#111EXPRIVIA000 - EXPRIVIA - AURORA - 2
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/AURORA/2/report-checklist.xlsx
+++ b/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/AURORA/2/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exprivia.sharepoint.com/sites/DFEH-PS-FSE2.0adeguamenti/Documenti condivisi/Documenti Accreditamento/Accreditamento AURORA-PS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exprivia.sharepoint.com/sites/DFEH-PS-FSE2.0adeguamenti/Documenti condivisi/Documenti Accreditamento/Accreditamento AURORA-PS/FILES/Accreditamento Gateway 04 aprile 2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{DC21B97C-41D4-4328-A083-28BBC17E4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ACD091D-C99E-4B86-8C06-F6EEF9FA157D}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="8_{DC21B97C-41D4-4328-A083-28BBC17E4B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76F1FD58-20A7-4D30-A74B-3DE54210490B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="371">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -492,15 +492,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>2023-03-17T10:41:23Z</t>
-  </si>
-  <si>
-    <t>7d5b6c81d1222a40</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4.4.ad48a59345aab41a9b8e3ab5b532c6258b943a33517501d5f024773a25e56006.d483c47164^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -608,16 +599,7 @@
     <t>VALIDAZIONE_TOKEN_JWT_VPS_KO</t>
   </si>
   <si>
-    <t>2023-03-17T15:35:35Z</t>
-  </si>
-  <si>
-    <t>187624cec5a6b8ec</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
-  </si>
-  <si>
-    <t>{"traceID":"187624cec5a6b8ec","spanID":"187624cec5a6b8ec","type":"/msg/jwt-validation","title":"Campo token JWT non valido.","detail":"Il campo action_id non è valorizzato","status":403,"instance":"/jwt-mandatory-field-missing","workflowInstanceId":"UNKNOWN_WORKFLOW_ID"}</t>
   </si>
   <si>
     <t>Segnalato tramite sistema di monitoraggio</t>
@@ -693,6 +675,9 @@
     <t>2ec8949dff7cfa7a</t>
   </si>
   <si>
+    <t>Forzato errore per valorizzazione JWT con campo sub non coeerente con CF utente che fa richiesta servizio interoperabilità</t>
+  </si>
+  <si>
     <t>{"traceID":"2ec8949dff7cfa7a","spanID":"2ec8949dff7cfa7a","type":"/msg/jwt-validation","title":"Campo token JWT non valido.","detail":"Il codice fiscale nel campo sub non è corretto","status":403,"instance":"/jwt-mandatory-field-malformed","workflowInstanceId":"UNKNOWN_WORKFLOW_ID"}</t>
   </si>
   <si>
@@ -1463,6 +1448,9 @@
     <t>2.16.840.1.113883.2.9.2.30.4.4.0cb56f860602a75fdbb9f59f7fe0ab0659281fb0c2e10d72506a705e28bd7292.bb26293529^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
+    <t>Da configurazione prima di dimettere modificare la trascodifica del dizionario</t>
+  </si>
+  <si>
     <t>{"traceID":"c13c4e79d940f8eb","spanID":"c13c4e79d940f8eb","type":"/msg/vocabulary","title":"Errore vocabolario.","detail":"Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.2.9.6.1.54.6, Codes: Z]","status":400,"instance":"/validation/error","workflowInstanceId":"2.16.840.1.113883.2.9.2.30.4.4.0cb56f860602a75fdbb9f59f7fe0ab0659281fb0c2e10d72506a705e28bd7292.bb26293529^^^^urn:ihe:iti:xdw:2013:workflowInstanceId"}</t>
   </si>
   <si>
@@ -1572,6 +1560,18 @@
   </si>
   <si>
     <t>subject_application_version: 2</t>
+  </si>
+  <si>
+    <t>2023-04-04T17:53:00Z</t>
+  </si>
+  <si>
+    <t>120417b413274319</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.4.4.1a8c5333ef29baca2cb1076068d4b2ef3514755b69f3585390f85570a6bafbb4.e1fb3ab805^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I campi del token JWT possono essere valorizzati in maniera errata ma non possono essere mancanti. </t>
   </si>
 </sst>
 </file>
@@ -3663,7 +3663,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomRight" activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="B2" s="47"/>
       <c r="C2" s="48" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D2" s="47"/>
       <c r="F2" s="23"/>
@@ -3739,7 +3739,7 @@
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="55" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D3" s="47"/>
       <c r="F3" s="23"/>
@@ -3762,7 +3762,7 @@
       <c r="A4" s="51"/>
       <c r="B4" s="52"/>
       <c r="C4" s="55" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D4" s="47"/>
       <c r="E4" s="26"/>
@@ -3786,7 +3786,7 @@
       <c r="A5" s="53"/>
       <c r="B5" s="54"/>
       <c r="C5" s="55" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D5" s="47"/>
       <c r="F5" s="23"/>
@@ -4655,19 +4655,19 @@
         <v>91</v>
       </c>
       <c r="F31" s="34">
-        <v>45002</v>
+        <v>45020</v>
       </c>
       <c r="G31" s="35" t="s">
+        <v>367</v>
+      </c>
+      <c r="H31" s="35" t="s">
+        <v>368</v>
+      </c>
+      <c r="I31" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="J31" s="36" t="s">
         <v>92</v>
-      </c>
-      <c r="H31" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="I31" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="J31" s="36" t="s">
-        <v>95</v>
       </c>
       <c r="K31" s="36"/>
       <c r="L31" s="36"/>
@@ -4693,20 +4693,20 @@
         <v>89</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="35"/>
       <c r="H32" s="35"/>
       <c r="I32" s="35"/>
       <c r="J32" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K32" s="36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L32" s="36"/>
       <c r="M32" s="36"/>
@@ -4731,20 +4731,20 @@
         <v>89</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="35"/>
       <c r="H33" s="35"/>
       <c r="I33" s="35"/>
       <c r="J33" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K33" s="36" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L33" s="36"/>
       <c r="M33" s="36"/>
@@ -4769,20 +4769,20 @@
         <v>89</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="35"/>
       <c r="H34" s="35"/>
       <c r="I34" s="35"/>
       <c r="J34" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K34" s="36" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L34" s="36"/>
       <c r="M34" s="36"/>
@@ -4807,10 +4807,10 @@
         <v>41</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="35"/>
@@ -4827,7 +4827,7 @@
       <c r="R35" s="39"/>
       <c r="S35" s="37"/>
       <c r="T35" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4841,10 +4841,10 @@
         <v>53</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E36" s="33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="35"/>
@@ -4861,7 +4861,7 @@
       <c r="R36" s="39"/>
       <c r="S36" s="37"/>
       <c r="T36" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4875,10 +4875,10 @@
         <v>62</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E37" s="33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="35"/>
@@ -4895,7 +4895,7 @@
       <c r="R37" s="39"/>
       <c r="S37" s="37"/>
       <c r="T37" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4909,10 +4909,10 @@
         <v>71</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="35"/>
@@ -4929,7 +4929,7 @@
       <c r="R38" s="39"/>
       <c r="S38" s="37"/>
       <c r="T38" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4943,10 +4943,10 @@
         <v>80</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E39" s="33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F39" s="34"/>
       <c r="G39" s="35"/>
@@ -4963,10 +4963,10 @@
       <c r="R39" s="39"/>
       <c r="S39" s="37"/>
       <c r="T39" s="40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="31">
         <v>35</v>
       </c>
@@ -4977,47 +4977,31 @@
         <v>89</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E40" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="F40" s="34">
-        <v>45002</v>
-      </c>
-      <c r="G40" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="H40" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="I40" s="35" t="s">
-        <v>116</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="F40" s="34"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
       <c r="J40" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="M40" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="N40" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="O40" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="P40" s="36" t="s">
-        <v>118</v>
-      </c>
+      <c r="K40" s="36" t="s">
+        <v>370</v>
+      </c>
+      <c r="L40" s="36"/>
+      <c r="M40" s="36"/>
+      <c r="N40" s="36"/>
+      <c r="O40" s="36"/>
+      <c r="P40" s="36"/>
       <c r="Q40" s="36"/>
       <c r="R40" s="39"/>
       <c r="S40" s="37"/>
       <c r="T40" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5031,10 +5015,10 @@
         <v>41</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E41" s="33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F41" s="34"/>
       <c r="G41" s="35"/>
@@ -5051,7 +5035,7 @@
       <c r="R41" s="39"/>
       <c r="S41" s="37"/>
       <c r="T41" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5065,10 +5049,10 @@
         <v>53</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E42" s="33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F42" s="34"/>
       <c r="G42" s="35"/>
@@ -5085,7 +5069,7 @@
       <c r="R42" s="39"/>
       <c r="S42" s="37"/>
       <c r="T42" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5099,10 +5083,10 @@
         <v>62</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F43" s="34"/>
       <c r="G43" s="35"/>
@@ -5119,7 +5103,7 @@
       <c r="R43" s="39"/>
       <c r="S43" s="37"/>
       <c r="T43" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5133,10 +5117,10 @@
         <v>71</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E44" s="33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F44" s="34"/>
       <c r="G44" s="35"/>
@@ -5153,7 +5137,7 @@
       <c r="R44" s="39"/>
       <c r="S44" s="37"/>
       <c r="T44" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5167,10 +5151,10 @@
         <v>80</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E45" s="33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F45" s="34"/>
       <c r="G45" s="35"/>
@@ -5187,7 +5171,7 @@
       <c r="R45" s="39"/>
       <c r="S45" s="37"/>
       <c r="T45" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5201,47 +5185,49 @@
         <v>89</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F46" s="34">
         <v>45002</v>
       </c>
       <c r="G46" s="35" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H46" s="35" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="I46" s="35" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J46" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="K46" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="L46" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="K46" s="36"/>
-      <c r="L46" s="36" t="s">
-        <v>98</v>
-      </c>
       <c r="M46" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N46" s="36" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="O46" s="36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="P46" s="36" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="Q46" s="36"/>
       <c r="R46" s="39"/>
       <c r="S46" s="37"/>
       <c r="T46" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5255,10 +5241,10 @@
         <v>41</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E47" s="33" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F47" s="34"/>
       <c r="G47" s="35"/>
@@ -5273,11 +5259,11 @@
       <c r="P47" s="36"/>
       <c r="Q47" s="36"/>
       <c r="R47" s="39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S47" s="37"/>
       <c r="T47" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5291,10 +5277,10 @@
         <v>53</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F48" s="34"/>
       <c r="G48" s="35"/>
@@ -5309,11 +5295,11 @@
       <c r="P48" s="36"/>
       <c r="Q48" s="36"/>
       <c r="R48" s="39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S48" s="37"/>
       <c r="T48" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5327,10 +5313,10 @@
         <v>62</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E49" s="33" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F49" s="34"/>
       <c r="G49" s="35"/>
@@ -5345,11 +5331,11 @@
       <c r="P49" s="36"/>
       <c r="Q49" s="36"/>
       <c r="R49" s="39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S49" s="37"/>
       <c r="T49" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5363,10 +5349,10 @@
         <v>71</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F50" s="34"/>
       <c r="G50" s="35"/>
@@ -5381,11 +5367,11 @@
       <c r="P50" s="36"/>
       <c r="Q50" s="36"/>
       <c r="R50" s="39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S50" s="37"/>
       <c r="T50" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5399,10 +5385,10 @@
         <v>80</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E51" s="33" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F51" s="34"/>
       <c r="G51" s="35"/>
@@ -5417,11 +5403,11 @@
       <c r="P51" s="36"/>
       <c r="Q51" s="36"/>
       <c r="R51" s="39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S51" s="37"/>
       <c r="T51" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5435,10 +5421,10 @@
         <v>89</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F52" s="34">
         <v>45002</v>
@@ -5447,31 +5433,31 @@
       <c r="H52" s="35"/>
       <c r="I52" s="35"/>
       <c r="J52" s="36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K52" s="36"/>
       <c r="L52" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="M52" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N52" s="36" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="O52" s="36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="P52" s="36" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="Q52" s="36"/>
       <c r="R52" s="39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="S52" s="37"/>
       <c r="T52" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5485,10 +5471,10 @@
         <v>41</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F53" s="34"/>
       <c r="G53" s="35"/>
@@ -5505,7 +5491,7 @@
       <c r="R53" s="39"/>
       <c r="S53" s="37"/>
       <c r="T53" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5519,10 +5505,10 @@
         <v>41</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F54" s="34"/>
       <c r="G54" s="35"/>
@@ -5539,7 +5525,7 @@
       <c r="R54" s="39"/>
       <c r="S54" s="37"/>
       <c r="T54" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5553,10 +5539,10 @@
         <v>41</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F55" s="34"/>
       <c r="G55" s="35"/>
@@ -5573,7 +5559,7 @@
       <c r="R55" s="39"/>
       <c r="S55" s="37"/>
       <c r="T55" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5587,10 +5573,10 @@
         <v>41</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F56" s="34"/>
       <c r="G56" s="35"/>
@@ -5607,7 +5593,7 @@
       <c r="R56" s="39"/>
       <c r="S56" s="37"/>
       <c r="T56" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5621,10 +5607,10 @@
         <v>41</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E57" s="33" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F57" s="34"/>
       <c r="G57" s="35"/>
@@ -5641,7 +5627,7 @@
       <c r="R57" s="39"/>
       <c r="S57" s="37"/>
       <c r="T57" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5655,10 +5641,10 @@
         <v>41</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E58" s="33" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F58" s="34"/>
       <c r="G58" s="35"/>
@@ -5675,7 +5661,7 @@
       <c r="R58" s="39"/>
       <c r="S58" s="37"/>
       <c r="T58" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5689,10 +5675,10 @@
         <v>41</v>
       </c>
       <c r="D59" s="32" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E59" s="33" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F59" s="34"/>
       <c r="G59" s="35"/>
@@ -5709,7 +5695,7 @@
       <c r="R59" s="39"/>
       <c r="S59" s="37"/>
       <c r="T59" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5723,10 +5709,10 @@
         <v>41</v>
       </c>
       <c r="D60" s="32" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E60" s="33" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F60" s="34"/>
       <c r="G60" s="35"/>
@@ -5743,7 +5729,7 @@
       <c r="R60" s="39"/>
       <c r="S60" s="37"/>
       <c r="T60" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5757,10 +5743,10 @@
         <v>41</v>
       </c>
       <c r="D61" s="32" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E61" s="33" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F61" s="34"/>
       <c r="G61" s="35"/>
@@ -5777,7 +5763,7 @@
       <c r="R61" s="39"/>
       <c r="S61" s="37"/>
       <c r="T61" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5791,10 +5777,10 @@
         <v>41</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E62" s="33" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F62" s="34"/>
       <c r="G62" s="35"/>
@@ -5811,7 +5797,7 @@
       <c r="R62" s="39"/>
       <c r="S62" s="37"/>
       <c r="T62" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5825,10 +5811,10 @@
         <v>41</v>
       </c>
       <c r="D63" s="32" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E63" s="33" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F63" s="34"/>
       <c r="G63" s="35"/>
@@ -5845,7 +5831,7 @@
       <c r="R63" s="39"/>
       <c r="S63" s="37"/>
       <c r="T63" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5859,10 +5845,10 @@
         <v>53</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E64" s="33" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F64" s="34"/>
       <c r="G64" s="35"/>
@@ -5879,7 +5865,7 @@
       <c r="R64" s="39"/>
       <c r="S64" s="37"/>
       <c r="T64" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5893,10 +5879,10 @@
         <v>53</v>
       </c>
       <c r="D65" s="32" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E65" s="33" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F65" s="34"/>
       <c r="G65" s="35"/>
@@ -5913,7 +5899,7 @@
       <c r="R65" s="39"/>
       <c r="S65" s="37"/>
       <c r="T65" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5927,10 +5913,10 @@
         <v>53</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E66" s="33" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F66" s="34"/>
       <c r="G66" s="35"/>
@@ -5947,7 +5933,7 @@
       <c r="R66" s="39"/>
       <c r="S66" s="37"/>
       <c r="T66" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5961,10 +5947,10 @@
         <v>53</v>
       </c>
       <c r="D67" s="32" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E67" s="33" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F67" s="34"/>
       <c r="G67" s="35"/>
@@ -5981,7 +5967,7 @@
       <c r="R67" s="39"/>
       <c r="S67" s="37"/>
       <c r="T67" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5995,10 +5981,10 @@
         <v>53</v>
       </c>
       <c r="D68" s="32" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E68" s="33" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F68" s="34"/>
       <c r="G68" s="35"/>
@@ -6015,7 +6001,7 @@
       <c r="R68" s="39"/>
       <c r="S68" s="37"/>
       <c r="T68" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6029,10 +6015,10 @@
         <v>53</v>
       </c>
       <c r="D69" s="32" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E69" s="33" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F69" s="34"/>
       <c r="G69" s="35"/>
@@ -6049,7 +6035,7 @@
       <c r="R69" s="39"/>
       <c r="S69" s="37"/>
       <c r="T69" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6063,10 +6049,10 @@
         <v>53</v>
       </c>
       <c r="D70" s="32" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E70" s="33" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F70" s="34"/>
       <c r="G70" s="35"/>
@@ -6083,7 +6069,7 @@
       <c r="R70" s="39"/>
       <c r="S70" s="37"/>
       <c r="T70" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6097,10 +6083,10 @@
         <v>53</v>
       </c>
       <c r="D71" s="32" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E71" s="33" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F71" s="34"/>
       <c r="G71" s="35"/>
@@ -6117,7 +6103,7 @@
       <c r="R71" s="39"/>
       <c r="S71" s="37"/>
       <c r="T71" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6131,10 +6117,10 @@
         <v>53</v>
       </c>
       <c r="D72" s="32" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E72" s="33" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F72" s="34"/>
       <c r="G72" s="35"/>
@@ -6151,7 +6137,7 @@
       <c r="R72" s="39"/>
       <c r="S72" s="37"/>
       <c r="T72" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6165,10 +6151,10 @@
         <v>53</v>
       </c>
       <c r="D73" s="32" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E73" s="33" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F73" s="34"/>
       <c r="G73" s="35"/>
@@ -6185,7 +6171,7 @@
       <c r="R73" s="39"/>
       <c r="S73" s="37"/>
       <c r="T73" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6199,10 +6185,10 @@
         <v>53</v>
       </c>
       <c r="D74" s="32" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E74" s="33" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F74" s="34"/>
       <c r="G74" s="35"/>
@@ -6219,7 +6205,7 @@
       <c r="R74" s="39"/>
       <c r="S74" s="37"/>
       <c r="T74" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6233,10 +6219,10 @@
         <v>53</v>
       </c>
       <c r="D75" s="32" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E75" s="33" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F75" s="34"/>
       <c r="G75" s="35"/>
@@ -6253,7 +6239,7 @@
       <c r="R75" s="39"/>
       <c r="S75" s="37"/>
       <c r="T75" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6267,10 +6253,10 @@
         <v>62</v>
       </c>
       <c r="D76" s="32" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E76" s="33" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F76" s="34"/>
       <c r="G76" s="35"/>
@@ -6287,7 +6273,7 @@
       <c r="R76" s="39"/>
       <c r="S76" s="37"/>
       <c r="T76" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6301,10 +6287,10 @@
         <v>62</v>
       </c>
       <c r="D77" s="32" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E77" s="33" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F77" s="34"/>
       <c r="G77" s="35"/>
@@ -6321,7 +6307,7 @@
       <c r="R77" s="39"/>
       <c r="S77" s="37"/>
       <c r="T77" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6335,10 +6321,10 @@
         <v>62</v>
       </c>
       <c r="D78" s="32" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E78" s="33" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F78" s="34"/>
       <c r="G78" s="35"/>
@@ -6355,7 +6341,7 @@
       <c r="R78" s="39"/>
       <c r="S78" s="37"/>
       <c r="T78" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6369,10 +6355,10 @@
         <v>62</v>
       </c>
       <c r="D79" s="32" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E79" s="33" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F79" s="34"/>
       <c r="G79" s="35"/>
@@ -6389,7 +6375,7 @@
       <c r="R79" s="39"/>
       <c r="S79" s="37"/>
       <c r="T79" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6403,10 +6389,10 @@
         <v>62</v>
       </c>
       <c r="D80" s="32" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E80" s="33" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F80" s="34"/>
       <c r="G80" s="35"/>
@@ -6423,7 +6409,7 @@
       <c r="R80" s="39"/>
       <c r="S80" s="37"/>
       <c r="T80" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6437,10 +6423,10 @@
         <v>62</v>
       </c>
       <c r="D81" s="32" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E81" s="33" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F81" s="34"/>
       <c r="G81" s="35"/>
@@ -6457,7 +6443,7 @@
       <c r="R81" s="39"/>
       <c r="S81" s="37"/>
       <c r="T81" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6471,10 +6457,10 @@
         <v>62</v>
       </c>
       <c r="D82" s="32" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E82" s="33" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F82" s="34"/>
       <c r="G82" s="35"/>
@@ -6491,7 +6477,7 @@
       <c r="R82" s="39"/>
       <c r="S82" s="37"/>
       <c r="T82" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6505,10 +6491,10 @@
         <v>62</v>
       </c>
       <c r="D83" s="32" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E83" s="33" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F83" s="34"/>
       <c r="G83" s="35"/>
@@ -6525,7 +6511,7 @@
       <c r="R83" s="39"/>
       <c r="S83" s="37"/>
       <c r="T83" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6539,10 +6525,10 @@
         <v>62</v>
       </c>
       <c r="D84" s="32" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E84" s="33" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F84" s="34"/>
       <c r="G84" s="35"/>
@@ -6559,7 +6545,7 @@
       <c r="R84" s="39"/>
       <c r="S84" s="37"/>
       <c r="T84" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6573,10 +6559,10 @@
         <v>62</v>
       </c>
       <c r="D85" s="32" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E85" s="33" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F85" s="34"/>
       <c r="G85" s="35"/>
@@ -6593,7 +6579,7 @@
       <c r="R85" s="39"/>
       <c r="S85" s="37"/>
       <c r="T85" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="86" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6607,10 +6593,10 @@
         <v>62</v>
       </c>
       <c r="D86" s="32" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E86" s="33" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F86" s="34"/>
       <c r="G86" s="35"/>
@@ -6627,7 +6613,7 @@
       <c r="R86" s="39"/>
       <c r="S86" s="37"/>
       <c r="T86" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="87" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6641,10 +6627,10 @@
         <v>62</v>
       </c>
       <c r="D87" s="32" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E87" s="33" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F87" s="34"/>
       <c r="G87" s="35"/>
@@ -6661,7 +6647,7 @@
       <c r="R87" s="39"/>
       <c r="S87" s="37"/>
       <c r="T87" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="88" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6675,10 +6661,10 @@
         <v>62</v>
       </c>
       <c r="D88" s="32" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E88" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F88" s="34"/>
       <c r="G88" s="35"/>
@@ -6695,7 +6681,7 @@
       <c r="R88" s="39"/>
       <c r="S88" s="37"/>
       <c r="T88" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6709,10 +6695,10 @@
         <v>62</v>
       </c>
       <c r="D89" s="32" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E89" s="33" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F89" s="34"/>
       <c r="G89" s="35"/>
@@ -6729,7 +6715,7 @@
       <c r="R89" s="39"/>
       <c r="S89" s="37"/>
       <c r="T89" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="90" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6743,10 +6729,10 @@
         <v>62</v>
       </c>
       <c r="D90" s="32" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E90" s="33" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F90" s="34"/>
       <c r="G90" s="35"/>
@@ -6763,7 +6749,7 @@
       <c r="R90" s="39"/>
       <c r="S90" s="37"/>
       <c r="T90" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6777,10 +6763,10 @@
         <v>62</v>
       </c>
       <c r="D91" s="32" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E91" s="33" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F91" s="34"/>
       <c r="G91" s="35"/>
@@ -6797,7 +6783,7 @@
       <c r="R91" s="39"/>
       <c r="S91" s="37"/>
       <c r="T91" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6811,10 +6797,10 @@
         <v>62</v>
       </c>
       <c r="D92" s="32" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E92" s="33" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F92" s="34"/>
       <c r="G92" s="35"/>
@@ -6831,7 +6817,7 @@
       <c r="R92" s="39"/>
       <c r="S92" s="37"/>
       <c r="T92" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6845,10 +6831,10 @@
         <v>62</v>
       </c>
       <c r="D93" s="32" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E93" s="33" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F93" s="34"/>
       <c r="G93" s="35"/>
@@ -6865,7 +6851,7 @@
       <c r="R93" s="39"/>
       <c r="S93" s="37"/>
       <c r="T93" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6879,10 +6865,10 @@
         <v>62</v>
       </c>
       <c r="D94" s="32" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E94" s="33" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F94" s="34"/>
       <c r="G94" s="35"/>
@@ -6899,7 +6885,7 @@
       <c r="R94" s="39"/>
       <c r="S94" s="37"/>
       <c r="T94" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6913,10 +6899,10 @@
         <v>71</v>
       </c>
       <c r="D95" s="32" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E95" s="33" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F95" s="34"/>
       <c r="G95" s="35"/>
@@ -6933,7 +6919,7 @@
       <c r="R95" s="39"/>
       <c r="S95" s="37"/>
       <c r="T95" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6947,10 +6933,10 @@
         <v>71</v>
       </c>
       <c r="D96" s="32" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E96" s="33" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F96" s="34"/>
       <c r="G96" s="35"/>
@@ -6967,7 +6953,7 @@
       <c r="R96" s="39"/>
       <c r="S96" s="37"/>
       <c r="T96" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6981,10 +6967,10 @@
         <v>71</v>
       </c>
       <c r="D97" s="32" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E97" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F97" s="34"/>
       <c r="G97" s="35"/>
@@ -7001,7 +6987,7 @@
       <c r="R97" s="39"/>
       <c r="S97" s="37"/>
       <c r="T97" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="98" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7015,10 +7001,10 @@
         <v>71</v>
       </c>
       <c r="D98" s="32" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E98" s="33" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F98" s="34"/>
       <c r="G98" s="35"/>
@@ -7035,7 +7021,7 @@
       <c r="R98" s="39"/>
       <c r="S98" s="37"/>
       <c r="T98" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7049,10 +7035,10 @@
         <v>71</v>
       </c>
       <c r="D99" s="32" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E99" s="33" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F99" s="34"/>
       <c r="G99" s="35"/>
@@ -7069,7 +7055,7 @@
       <c r="R99" s="39"/>
       <c r="S99" s="37"/>
       <c r="T99" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7083,10 +7069,10 @@
         <v>71</v>
       </c>
       <c r="D100" s="32" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E100" s="33" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F100" s="34"/>
       <c r="G100" s="35"/>
@@ -7103,7 +7089,7 @@
       <c r="R100" s="39"/>
       <c r="S100" s="37"/>
       <c r="T100" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7117,10 +7103,10 @@
         <v>71</v>
       </c>
       <c r="D101" s="32" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E101" s="33" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F101" s="34"/>
       <c r="G101" s="35"/>
@@ -7137,7 +7123,7 @@
       <c r="R101" s="39"/>
       <c r="S101" s="37"/>
       <c r="T101" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="102" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7151,10 +7137,10 @@
         <v>71</v>
       </c>
       <c r="D102" s="32" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E102" s="33" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F102" s="34"/>
       <c r="G102" s="35"/>
@@ -7171,7 +7157,7 @@
       <c r="R102" s="39"/>
       <c r="S102" s="37"/>
       <c r="T102" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="103" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7185,10 +7171,10 @@
         <v>71</v>
       </c>
       <c r="D103" s="32" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E103" s="33" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F103" s="34"/>
       <c r="G103" s="35"/>
@@ -7205,7 +7191,7 @@
       <c r="R103" s="39"/>
       <c r="S103" s="37"/>
       <c r="T103" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="104" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7219,10 +7205,10 @@
         <v>71</v>
       </c>
       <c r="D104" s="32" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E104" s="33" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F104" s="34"/>
       <c r="G104" s="35"/>
@@ -7239,7 +7225,7 @@
       <c r="R104" s="39"/>
       <c r="S104" s="37"/>
       <c r="T104" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="105" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7253,10 +7239,10 @@
         <v>71</v>
       </c>
       <c r="D105" s="32" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E105" s="33" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F105" s="34"/>
       <c r="G105" s="35"/>
@@ -7273,7 +7259,7 @@
       <c r="R105" s="39"/>
       <c r="S105" s="37"/>
       <c r="T105" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="106" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7287,10 +7273,10 @@
         <v>71</v>
       </c>
       <c r="D106" s="32" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E106" s="33" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F106" s="34"/>
       <c r="G106" s="35"/>
@@ -7307,7 +7293,7 @@
       <c r="R106" s="39"/>
       <c r="S106" s="37"/>
       <c r="T106" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="107" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7321,10 +7307,10 @@
         <v>71</v>
       </c>
       <c r="D107" s="32" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E107" s="33" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F107" s="34"/>
       <c r="G107" s="35"/>
@@ -7341,7 +7327,7 @@
       <c r="R107" s="39"/>
       <c r="S107" s="37"/>
       <c r="T107" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7355,10 +7341,10 @@
         <v>80</v>
       </c>
       <c r="D108" s="32" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E108" s="33" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F108" s="34"/>
       <c r="G108" s="35"/>
@@ -7375,7 +7361,7 @@
       <c r="R108" s="39"/>
       <c r="S108" s="37"/>
       <c r="T108" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="109" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7389,10 +7375,10 @@
         <v>80</v>
       </c>
       <c r="D109" s="32" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E109" s="33" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F109" s="34"/>
       <c r="G109" s="35"/>
@@ -7409,7 +7395,7 @@
       <c r="R109" s="39"/>
       <c r="S109" s="37"/>
       <c r="T109" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7423,10 +7409,10 @@
         <v>80</v>
       </c>
       <c r="D110" s="32" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="E110" s="33" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F110" s="34"/>
       <c r="G110" s="35"/>
@@ -7443,7 +7429,7 @@
       <c r="R110" s="39"/>
       <c r="S110" s="37"/>
       <c r="T110" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:20" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7457,10 +7443,10 @@
         <v>80</v>
       </c>
       <c r="D111" s="32" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E111" s="33" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F111" s="34"/>
       <c r="G111" s="35"/>
@@ -7477,7 +7463,7 @@
       <c r="R111" s="39"/>
       <c r="S111" s="37"/>
       <c r="T111" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="112" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7491,10 +7477,10 @@
         <v>80</v>
       </c>
       <c r="D112" s="32" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="E112" s="33" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="F112" s="34"/>
       <c r="G112" s="35"/>
@@ -7511,7 +7497,7 @@
       <c r="R112" s="39"/>
       <c r="S112" s="37"/>
       <c r="T112" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7525,10 +7511,10 @@
         <v>80</v>
       </c>
       <c r="D113" s="32" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="E113" s="33" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="F113" s="34"/>
       <c r="G113" s="35"/>
@@ -7545,7 +7531,7 @@
       <c r="R113" s="39"/>
       <c r="S113" s="37"/>
       <c r="T113" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="114" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7559,10 +7545,10 @@
         <v>80</v>
       </c>
       <c r="D114" s="32" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E114" s="33" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="F114" s="34"/>
       <c r="G114" s="35"/>
@@ -7579,7 +7565,7 @@
       <c r="R114" s="39"/>
       <c r="S114" s="37"/>
       <c r="T114" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7593,10 +7579,10 @@
         <v>80</v>
       </c>
       <c r="D115" s="32" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="E115" s="33" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F115" s="34"/>
       <c r="G115" s="35"/>
@@ -7613,7 +7599,7 @@
       <c r="R115" s="39"/>
       <c r="S115" s="37"/>
       <c r="T115" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="116" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7627,10 +7613,10 @@
         <v>80</v>
       </c>
       <c r="D116" s="32" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E116" s="33" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="F116" s="34"/>
       <c r="G116" s="35"/>
@@ -7647,7 +7633,7 @@
       <c r="R116" s="39"/>
       <c r="S116" s="37"/>
       <c r="T116" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="117" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7661,10 +7647,10 @@
         <v>80</v>
       </c>
       <c r="D117" s="32" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="E117" s="33" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F117" s="34"/>
       <c r="G117" s="35"/>
@@ -7681,7 +7667,7 @@
       <c r="R117" s="39"/>
       <c r="S117" s="37"/>
       <c r="T117" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="118" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7695,10 +7681,10 @@
         <v>80</v>
       </c>
       <c r="D118" s="32" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="E118" s="33" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="F118" s="34"/>
       <c r="G118" s="35"/>
@@ -7715,7 +7701,7 @@
       <c r="R118" s="39"/>
       <c r="S118" s="37"/>
       <c r="T118" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="119" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7729,10 +7715,10 @@
         <v>80</v>
       </c>
       <c r="D119" s="32" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="E119" s="33" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="F119" s="34"/>
       <c r="G119" s="35"/>
@@ -7749,7 +7735,7 @@
       <c r="R119" s="39"/>
       <c r="S119" s="37"/>
       <c r="T119" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="120" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7763,10 +7749,10 @@
         <v>80</v>
       </c>
       <c r="D120" s="32" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E120" s="33" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="F120" s="34"/>
       <c r="G120" s="35"/>
@@ -7783,7 +7769,7 @@
       <c r="R120" s="39"/>
       <c r="S120" s="37"/>
       <c r="T120" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="121" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7797,10 +7783,10 @@
         <v>80</v>
       </c>
       <c r="D121" s="32" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E121" s="33" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="F121" s="34"/>
       <c r="G121" s="35"/>
@@ -7817,7 +7803,7 @@
       <c r="R121" s="39"/>
       <c r="S121" s="37"/>
       <c r="T121" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:20" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7831,10 +7817,10 @@
         <v>80</v>
       </c>
       <c r="D122" s="32" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E122" s="33" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="F122" s="34"/>
       <c r="G122" s="35"/>
@@ -7851,7 +7837,7 @@
       <c r="R122" s="39"/>
       <c r="S122" s="37"/>
       <c r="T122" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="123" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7865,20 +7851,20 @@
         <v>89</v>
       </c>
       <c r="D123" s="32" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E123" s="33" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F123" s="34"/>
       <c r="G123" s="35"/>
       <c r="H123" s="35"/>
       <c r="I123" s="35"/>
       <c r="J123" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K123" s="36" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="L123" s="36"/>
       <c r="M123" s="36"/>
@@ -7889,7 +7875,7 @@
       <c r="R123" s="39"/>
       <c r="S123" s="37"/>
       <c r="T123" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="124" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7903,20 +7889,20 @@
         <v>89</v>
       </c>
       <c r="D124" s="32" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E124" s="33" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F124" s="34"/>
       <c r="G124" s="35"/>
       <c r="H124" s="35"/>
       <c r="I124" s="35"/>
       <c r="J124" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K124" s="36" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="L124" s="36"/>
       <c r="M124" s="36"/>
@@ -7927,7 +7913,7 @@
       <c r="R124" s="39"/>
       <c r="S124" s="37"/>
       <c r="T124" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="125" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7941,20 +7927,20 @@
         <v>89</v>
       </c>
       <c r="D125" s="32" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="E125" s="33" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F125" s="34"/>
       <c r="G125" s="35"/>
       <c r="H125" s="35"/>
       <c r="I125" s="35"/>
       <c r="J125" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K125" s="36" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="L125" s="36"/>
       <c r="M125" s="36"/>
@@ -7965,7 +7951,7 @@
       <c r="R125" s="39"/>
       <c r="S125" s="37"/>
       <c r="T125" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="126" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7979,20 +7965,20 @@
         <v>89</v>
       </c>
       <c r="D126" s="32" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="E126" s="33" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F126" s="34"/>
       <c r="G126" s="35"/>
       <c r="H126" s="35"/>
       <c r="I126" s="35"/>
       <c r="J126" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K126" s="36" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="L126" s="36"/>
       <c r="M126" s="36"/>
@@ -8003,7 +7989,7 @@
       <c r="R126" s="39"/>
       <c r="S126" s="37"/>
       <c r="T126" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="127" spans="1:20" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8017,20 +8003,20 @@
         <v>89</v>
       </c>
       <c r="D127" s="32" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E127" s="33" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="F127" s="34"/>
       <c r="G127" s="35"/>
       <c r="H127" s="35"/>
       <c r="I127" s="35"/>
       <c r="J127" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K127" s="36" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="L127" s="36"/>
       <c r="M127" s="36"/>
@@ -8041,7 +8027,7 @@
       <c r="R127" s="39"/>
       <c r="S127" s="37"/>
       <c r="T127" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="128" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8055,20 +8041,20 @@
         <v>89</v>
       </c>
       <c r="D128" s="32" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="E128" s="33" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F128" s="34"/>
       <c r="G128" s="35"/>
       <c r="H128" s="35"/>
       <c r="I128" s="35"/>
       <c r="J128" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K128" s="36" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="L128" s="36"/>
       <c r="M128" s="36"/>
@@ -8079,7 +8065,7 @@
       <c r="R128" s="39"/>
       <c r="S128" s="37"/>
       <c r="T128" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="129" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8093,20 +8079,20 @@
         <v>89</v>
       </c>
       <c r="D129" s="32" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="E129" s="33" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F129" s="34"/>
       <c r="G129" s="35"/>
       <c r="H129" s="35"/>
       <c r="I129" s="35"/>
       <c r="J129" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K129" s="36" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="L129" s="36"/>
       <c r="M129" s="36"/>
@@ -8117,7 +8103,7 @@
       <c r="R129" s="39"/>
       <c r="S129" s="37"/>
       <c r="T129" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="130" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8131,20 +8117,20 @@
         <v>89</v>
       </c>
       <c r="D130" s="32" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E130" s="33" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F130" s="34"/>
       <c r="G130" s="35"/>
       <c r="H130" s="35"/>
       <c r="I130" s="35"/>
       <c r="J130" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K130" s="36" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="L130" s="36"/>
       <c r="M130" s="36"/>
@@ -8155,7 +8141,7 @@
       <c r="R130" s="39"/>
       <c r="S130" s="37"/>
       <c r="T130" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="131" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8169,20 +8155,20 @@
         <v>89</v>
       </c>
       <c r="D131" s="32" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E131" s="33" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="F131" s="34"/>
       <c r="G131" s="35"/>
       <c r="H131" s="35"/>
       <c r="I131" s="35"/>
       <c r="J131" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K131" s="36" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="L131" s="36"/>
       <c r="M131" s="36"/>
@@ -8193,7 +8179,7 @@
       <c r="R131" s="39"/>
       <c r="S131" s="37"/>
       <c r="T131" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="132" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8207,20 +8193,20 @@
         <v>89</v>
       </c>
       <c r="D132" s="32" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E132" s="33" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="F132" s="34"/>
       <c r="G132" s="35"/>
       <c r="H132" s="35"/>
       <c r="I132" s="35"/>
       <c r="J132" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K132" s="36" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="L132" s="36"/>
       <c r="M132" s="36"/>
@@ -8231,7 +8217,7 @@
       <c r="R132" s="39"/>
       <c r="S132" s="37"/>
       <c r="T132" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="133" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8245,20 +8231,20 @@
         <v>89</v>
       </c>
       <c r="D133" s="32" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E133" s="33" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F133" s="34"/>
       <c r="G133" s="35"/>
       <c r="H133" s="35"/>
       <c r="I133" s="35"/>
       <c r="J133" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K133" s="36" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="L133" s="36"/>
       <c r="M133" s="36"/>
@@ -8269,7 +8255,7 @@
       <c r="R133" s="39"/>
       <c r="S133" s="37"/>
       <c r="T133" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="134" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8283,20 +8269,20 @@
         <v>89</v>
       </c>
       <c r="D134" s="32" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E134" s="33" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F134" s="34"/>
       <c r="G134" s="35"/>
       <c r="H134" s="35"/>
       <c r="I134" s="35"/>
       <c r="J134" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K134" s="36" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="L134" s="36"/>
       <c r="M134" s="36"/>
@@ -8307,7 +8293,7 @@
       <c r="R134" s="39"/>
       <c r="S134" s="37"/>
       <c r="T134" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="135" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8321,20 +8307,20 @@
         <v>89</v>
       </c>
       <c r="D135" s="32" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E135" s="33" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="F135" s="34"/>
       <c r="G135" s="35"/>
       <c r="H135" s="35"/>
       <c r="I135" s="35"/>
       <c r="J135" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K135" s="36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L135" s="36"/>
       <c r="M135" s="36"/>
@@ -8345,7 +8331,7 @@
       <c r="R135" s="39"/>
       <c r="S135" s="37"/>
       <c r="T135" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="136" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8359,20 +8345,20 @@
         <v>89</v>
       </c>
       <c r="D136" s="32" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E136" s="33" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="F136" s="34"/>
       <c r="G136" s="35"/>
       <c r="H136" s="35"/>
       <c r="I136" s="35"/>
       <c r="J136" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K136" s="36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L136" s="36"/>
       <c r="M136" s="36"/>
@@ -8383,7 +8369,7 @@
       <c r="R136" s="39"/>
       <c r="S136" s="37"/>
       <c r="T136" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="137" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8397,20 +8383,20 @@
         <v>89</v>
       </c>
       <c r="D137" s="32" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E137" s="33" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F137" s="34"/>
       <c r="G137" s="35"/>
       <c r="H137" s="35"/>
       <c r="I137" s="35"/>
       <c r="J137" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K137" s="36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L137" s="36"/>
       <c r="M137" s="36"/>
@@ -8421,7 +8407,7 @@
       <c r="R137" s="39"/>
       <c r="S137" s="37"/>
       <c r="T137" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="138" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8435,20 +8421,20 @@
         <v>89</v>
       </c>
       <c r="D138" s="32" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E138" s="33" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F138" s="34"/>
       <c r="G138" s="35"/>
       <c r="H138" s="35"/>
       <c r="I138" s="35"/>
       <c r="J138" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K138" s="36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L138" s="36"/>
       <c r="M138" s="36"/>
@@ -8459,7 +8445,7 @@
       <c r="R138" s="39"/>
       <c r="S138" s="37"/>
       <c r="T138" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="139" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8473,20 +8459,20 @@
         <v>89</v>
       </c>
       <c r="D139" s="32" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="E139" s="33" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F139" s="34"/>
       <c r="G139" s="35"/>
       <c r="H139" s="35"/>
       <c r="I139" s="35"/>
       <c r="J139" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K139" s="36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L139" s="36"/>
       <c r="M139" s="36"/>
@@ -8497,7 +8483,7 @@
       <c r="R139" s="39"/>
       <c r="S139" s="37"/>
       <c r="T139" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="140" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8511,20 +8497,20 @@
         <v>89</v>
       </c>
       <c r="D140" s="32" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="E140" s="33" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F140" s="34"/>
       <c r="G140" s="35"/>
       <c r="H140" s="35"/>
       <c r="I140" s="35"/>
       <c r="J140" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K140" s="36" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="L140" s="36"/>
       <c r="M140" s="36"/>
@@ -8535,7 +8521,7 @@
       <c r="R140" s="39"/>
       <c r="S140" s="37"/>
       <c r="T140" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="141" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8549,20 +8535,20 @@
         <v>89</v>
       </c>
       <c r="D141" s="32" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E141" s="33" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F141" s="34"/>
       <c r="G141" s="35"/>
       <c r="H141" s="35"/>
       <c r="I141" s="35"/>
       <c r="J141" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K141" s="36" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="L141" s="36"/>
       <c r="M141" s="36"/>
@@ -8573,7 +8559,7 @@
       <c r="R141" s="39"/>
       <c r="S141" s="37"/>
       <c r="T141" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="142" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8587,20 +8573,20 @@
         <v>89</v>
       </c>
       <c r="D142" s="32" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E142" s="33" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="F142" s="34"/>
       <c r="G142" s="35"/>
       <c r="H142" s="35"/>
       <c r="I142" s="35"/>
       <c r="J142" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K142" s="36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L142" s="36"/>
       <c r="M142" s="36"/>
@@ -8611,7 +8597,7 @@
       <c r="R142" s="39"/>
       <c r="S142" s="37"/>
       <c r="T142" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="143" spans="1:20" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8625,47 +8611,49 @@
         <v>89</v>
       </c>
       <c r="D143" s="32" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="E143" s="33" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F143" s="34">
         <v>45002</v>
       </c>
       <c r="G143" s="35" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="H143" s="35" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="I143" s="35" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="J143" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="K143" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="L143" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="M143" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="K143" s="36"/>
-      <c r="L143" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="M143" s="36" t="s">
-        <v>98</v>
-      </c>
       <c r="N143" s="36" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="O143" s="36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="P143" s="36" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="Q143" s="36"/>
       <c r="R143" s="39"/>
       <c r="S143" s="37"/>
       <c r="T143" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="144" spans="1:20" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8679,47 +8667,49 @@
         <v>89</v>
       </c>
       <c r="D144" s="32" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E144" s="33" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F144" s="34">
         <v>45002</v>
       </c>
       <c r="G144" s="35" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="H144" s="35" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="I144" s="35" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="J144" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="K144" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="L144" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="M144" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="K144" s="36"/>
-      <c r="L144" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="M144" s="36" t="s">
-        <v>98</v>
-      </c>
       <c r="N144" s="36" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="O144" s="36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="P144" s="36" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="Q144" s="36"/>
       <c r="R144" s="39"/>
       <c r="S144" s="37"/>
       <c r="T144" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="145" spans="1:20" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8733,20 +8723,20 @@
         <v>89</v>
       </c>
       <c r="D145" s="32" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E145" s="33" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F145" s="34"/>
       <c r="G145" s="35"/>
       <c r="H145" s="35"/>
       <c r="I145" s="35"/>
       <c r="J145" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K145" s="36" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="L145" s="36"/>
       <c r="M145" s="36"/>
@@ -8757,7 +8747,7 @@
       <c r="R145" s="39"/>
       <c r="S145" s="37"/>
       <c r="T145" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="146" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8771,20 +8761,20 @@
         <v>89</v>
       </c>
       <c r="D146" s="32" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E146" s="33" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F146" s="34"/>
       <c r="G146" s="35"/>
       <c r="H146" s="35"/>
       <c r="I146" s="35"/>
       <c r="J146" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K146" s="36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L146" s="36"/>
       <c r="M146" s="36"/>
@@ -8795,7 +8785,7 @@
       <c r="R146" s="39"/>
       <c r="S146" s="37"/>
       <c r="T146" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="147" spans="1:20" ht="135" x14ac:dyDescent="0.25">
@@ -8809,20 +8799,20 @@
         <v>89</v>
       </c>
       <c r="D147" s="32" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E147" s="33" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F147" s="34"/>
       <c r="G147" s="35"/>
       <c r="H147" s="35"/>
       <c r="I147" s="35"/>
       <c r="J147" s="36" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="K147" s="36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L147" s="36"/>
       <c r="M147" s="36"/>
@@ -8833,7 +8823,7 @@
       <c r="R147" s="39"/>
       <c r="S147" s="37"/>
       <c r="T147" s="40" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.25">
@@ -23274,10 +23264,10 @@
         <v>21</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23285,13 +23275,13 @@
         <v>41</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23299,13 +23289,13 @@
         <v>53</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>352</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>355</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23313,13 +23303,13 @@
         <v>62</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23327,13 +23317,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23341,13 +23331,13 @@
         <v>80</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -23355,13 +23345,13 @@
         <v>89</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24384,18 +24374,18 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -25409,12 +25399,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -25423,7 +25407,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100794258E7DE47134588D45098EBDB60F8" ma:contentTypeVersion="4" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="2dbc010f7356a33b20da83a73eb190a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0bdf65ce-24cf-486b-995b-57ece8b70f4e" xmlns:ns3="c50f76eb-a136-4a5c-b9b3-fbcc59ed104d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bbb2aea3e03736235287e3873b29b8db" ns2:_="" ns3:_="">
     <xsd:import namespace="0bdf65ce-24cf-486b-995b-57ece8b70f4e"/>
@@ -25588,16 +25572,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -25605,7 +25586,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D2D0A0-F0AE-444C-8C04-2406B9171C25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25624,6 +25605,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
aggiunto caso1 ok VPS id24
commonName auth: "A1#111EXPRIVIA000"
subject_application_vendor: "exprivia"
subject_application_id: "aurora"
subject_application_version: "2"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/AURORA/2/report-checklist.xlsx
+++ b/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/AURORA/2/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exprivia.sharepoint.com/sites/DFEH-PS-FSE2.0adeguamenti/Documenti condivisi/Documenti Accreditamento/Accreditamento AURORA MERGE/2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{834C2443-3908-4C51-8BF0-AF8F336E4695}"/>
+  <xr:revisionPtr revIDLastSave="251" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03C6FE6E-4BC3-4516-B408-0A3BDCD8BB72}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2175" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="874">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -2533,10 +2533,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di una futura pubblicazione con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>l'applicativo non gestisce sezioni incongruenti.
-vedi iGithub ssue #263</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT2</t>
@@ -4124,6 +4120,15 @@
   </si>
   <si>
     <t>{"traceID":"fbc6eb6346f6e97b","spanID":"fbc6eb6346f6e97b","type":"/msg/jwt-validation","title":"Campo token JWT non valido.","detail":"Il codice fiscale nel campo sub non ? corretto","status":403,"instance":"/jwt-mandatory-field-malformed","workflowInstanceId":"UNKNOWN_WORKFLOW_ID"}</t>
+  </si>
+  <si>
+    <t>6fa853f7cd17c1bc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.4.4.03529d9ee5b30d69aac31f17980a5f1fb13e5eb7b029a4d4cec36e0b94e270f3.f4c85b3d37^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-05-12T12:49:55Z</t>
   </si>
 </sst>
 </file>
@@ -7122,9 +7127,9 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="J88" sqref="J88"/>
+      <selection pane="bottomLeft" activeCell="K207" sqref="K207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -10050,13 +10055,13 @@
         <v>45054</v>
       </c>
       <c r="G88" s="24" t="s">
+        <v>865</v>
+      </c>
+      <c r="H88" s="24" t="s">
         <v>866</v>
       </c>
-      <c r="H88" s="24" t="s">
+      <c r="I88" s="24" t="s">
         <v>867</v>
-      </c>
-      <c r="I88" s="24" t="s">
-        <v>868</v>
       </c>
       <c r="J88" s="25" t="s">
         <v>215</v>
@@ -14216,16 +14221,22 @@
       <c r="E207" s="39" t="s">
         <v>472</v>
       </c>
-      <c r="F207" s="40"/>
-      <c r="G207" s="41"/>
-      <c r="H207" s="41"/>
-      <c r="I207" s="41"/>
+      <c r="F207" s="40">
+        <v>45058</v>
+      </c>
+      <c r="G207" s="41" t="s">
+        <v>873</v>
+      </c>
+      <c r="H207" s="41" t="s">
+        <v>871</v>
+      </c>
+      <c r="I207" s="41" t="s">
+        <v>872</v>
+      </c>
       <c r="J207" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="K207" s="42" t="s">
-        <v>473</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="K207" s="42"/>
       <c r="L207" s="33"/>
       <c r="M207" s="33"/>
       <c r="N207" s="33"/>
@@ -14249,10 +14260,10 @@
         <v>76</v>
       </c>
       <c r="D208" s="38" t="s">
+        <v>473</v>
+      </c>
+      <c r="E208" s="39" t="s">
         <v>474</v>
-      </c>
-      <c r="E208" s="39" t="s">
-        <v>475</v>
       </c>
       <c r="F208" s="40"/>
       <c r="G208" s="41"/>
@@ -14262,7 +14273,7 @@
         <v>218</v>
       </c>
       <c r="K208" s="33" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L208" s="33"/>
       <c r="M208" s="33"/>
@@ -14287,10 +14298,10 @@
         <v>76</v>
       </c>
       <c r="D209" s="38" t="s">
+        <v>476</v>
+      </c>
+      <c r="E209" s="39" t="s">
         <v>477</v>
-      </c>
-      <c r="E209" s="39" t="s">
-        <v>478</v>
       </c>
       <c r="F209" s="40"/>
       <c r="G209" s="41"/>
@@ -14300,7 +14311,7 @@
         <v>218</v>
       </c>
       <c r="K209" s="33" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="L209" s="33"/>
       <c r="M209" s="33"/>
@@ -14325,10 +14336,10 @@
         <v>76</v>
       </c>
       <c r="D210" s="38" t="s">
+        <v>479</v>
+      </c>
+      <c r="E210" s="39" t="s">
         <v>480</v>
-      </c>
-      <c r="E210" s="39" t="s">
-        <v>481</v>
       </c>
       <c r="F210" s="40"/>
       <c r="G210" s="41"/>
@@ -14338,7 +14349,7 @@
         <v>218</v>
       </c>
       <c r="K210" s="33" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="L210" s="33"/>
       <c r="M210" s="33"/>
@@ -14363,7 +14374,7 @@
         <v>49</v>
       </c>
       <c r="D211" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E211" s="22" t="s">
         <v>291</v>
@@ -14397,10 +14408,10 @@
         <v>403</v>
       </c>
       <c r="D212" s="21" t="s">
+        <v>483</v>
+      </c>
+      <c r="E212" s="22" t="s">
         <v>484</v>
-      </c>
-      <c r="E212" s="22" t="s">
-        <v>485</v>
       </c>
       <c r="F212" s="23"/>
       <c r="G212" s="24"/>
@@ -14431,7 +14442,7 @@
         <v>85</v>
       </c>
       <c r="D213" s="21" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E213" s="22" t="s">
         <v>291</v>
@@ -14465,7 +14476,7 @@
         <v>61</v>
       </c>
       <c r="D214" s="21" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E214" s="22" t="s">
         <v>291</v>
@@ -14499,10 +14510,10 @@
         <v>403</v>
       </c>
       <c r="D215" s="21" t="s">
+        <v>487</v>
+      </c>
+      <c r="E215" s="22" t="s">
         <v>488</v>
-      </c>
-      <c r="E215" s="22" t="s">
-        <v>489</v>
       </c>
       <c r="F215" s="23"/>
       <c r="G215" s="24"/>
@@ -14533,7 +14544,7 @@
         <v>66</v>
       </c>
       <c r="D216" s="21" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E216" s="22" t="s">
         <v>291</v>
@@ -14567,7 +14578,7 @@
         <v>71</v>
       </c>
       <c r="D217" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E217" s="22" t="s">
         <v>291</v>
@@ -14601,10 +14612,10 @@
         <v>76</v>
       </c>
       <c r="D218" s="38" t="s">
+        <v>491</v>
+      </c>
+      <c r="E218" s="39" t="s">
         <v>492</v>
-      </c>
-      <c r="E218" s="39" t="s">
-        <v>493</v>
       </c>
       <c r="F218" s="40"/>
       <c r="G218" s="41"/>
@@ -14614,7 +14625,7 @@
         <v>218</v>
       </c>
       <c r="K218" s="33" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L218" s="33"/>
       <c r="M218" s="33"/>
@@ -14639,7 +14650,7 @@
         <v>49</v>
       </c>
       <c r="D219" s="21" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E219" s="22" t="s">
         <v>294</v>
@@ -14673,10 +14684,10 @@
         <v>403</v>
       </c>
       <c r="D220" s="21" t="s">
+        <v>495</v>
+      </c>
+      <c r="E220" s="22" t="s">
         <v>496</v>
-      </c>
-      <c r="E220" s="22" t="s">
-        <v>497</v>
       </c>
       <c r="F220" s="23"/>
       <c r="G220" s="24"/>
@@ -14707,7 +14718,7 @@
         <v>85</v>
       </c>
       <c r="D221" s="21" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E221" s="22" t="s">
         <v>294</v>
@@ -14741,7 +14752,7 @@
         <v>61</v>
       </c>
       <c r="D222" s="21" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E222" s="22" t="s">
         <v>294</v>
@@ -14775,10 +14786,10 @@
         <v>403</v>
       </c>
       <c r="D223" s="21" t="s">
+        <v>499</v>
+      </c>
+      <c r="E223" s="22" t="s">
         <v>500</v>
-      </c>
-      <c r="E223" s="22" t="s">
-        <v>501</v>
       </c>
       <c r="F223" s="23"/>
       <c r="G223" s="24"/>
@@ -14809,7 +14820,7 @@
         <v>66</v>
       </c>
       <c r="D224" s="21" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E224" s="22" t="s">
         <v>294</v>
@@ -14843,7 +14854,7 @@
         <v>71</v>
       </c>
       <c r="D225" s="21" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E225" s="22" t="s">
         <v>294</v>
@@ -14877,19 +14888,19 @@
         <v>76</v>
       </c>
       <c r="D226" s="38" t="s">
+        <v>503</v>
+      </c>
+      <c r="E226" s="39" t="s">
         <v>504</v>
-      </c>
-      <c r="E226" s="39" t="s">
-        <v>505</v>
       </c>
       <c r="F226" s="40">
         <v>45054</v>
       </c>
       <c r="G226" s="41" t="s">
+        <v>868</v>
+      </c>
+      <c r="H226" s="41" t="s">
         <v>869</v>
-      </c>
-      <c r="H226" s="41" t="s">
-        <v>870</v>
       </c>
       <c r="I226" s="41" t="s">
         <v>297</v>
@@ -14905,7 +14916,7 @@
         <v>218</v>
       </c>
       <c r="N226" s="33" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="O226" s="33" t="s">
         <v>215</v>
@@ -14931,7 +14942,7 @@
         <v>49</v>
       </c>
       <c r="D227" s="21" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E227" s="22" t="s">
         <v>300</v>
@@ -14967,10 +14978,10 @@
         <v>403</v>
       </c>
       <c r="D228" s="21" t="s">
+        <v>506</v>
+      </c>
+      <c r="E228" s="22" t="s">
         <v>507</v>
-      </c>
-      <c r="E228" s="22" t="s">
-        <v>508</v>
       </c>
       <c r="F228" s="23"/>
       <c r="G228" s="24"/>
@@ -15001,7 +15012,7 @@
         <v>85</v>
       </c>
       <c r="D229" s="21" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E229" s="22" t="s">
         <v>300</v>
@@ -15037,7 +15048,7 @@
         <v>61</v>
       </c>
       <c r="D230" s="21" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E230" s="22" t="s">
         <v>300</v>
@@ -15073,10 +15084,10 @@
         <v>403</v>
       </c>
       <c r="D231" s="21" t="s">
+        <v>510</v>
+      </c>
+      <c r="E231" s="22" t="s">
         <v>511</v>
-      </c>
-      <c r="E231" s="22" t="s">
-        <v>512</v>
       </c>
       <c r="F231" s="23"/>
       <c r="G231" s="24"/>
@@ -15107,7 +15118,7 @@
         <v>66</v>
       </c>
       <c r="D232" s="21" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E232" s="22" t="s">
         <v>300</v>
@@ -15143,7 +15154,7 @@
         <v>71</v>
       </c>
       <c r="D233" s="21" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E233" s="22" t="s">
         <v>300</v>
@@ -15179,7 +15190,7 @@
         <v>76</v>
       </c>
       <c r="D234" s="38" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E234" s="39" t="s">
         <v>300</v>
@@ -15227,10 +15238,10 @@
         <v>49</v>
       </c>
       <c r="D235" s="21" t="s">
+        <v>515</v>
+      </c>
+      <c r="E235" s="22" t="s">
         <v>516</v>
-      </c>
-      <c r="E235" s="22" t="s">
-        <v>517</v>
       </c>
       <c r="F235" s="23"/>
       <c r="G235" s="24"/>
@@ -15261,10 +15272,10 @@
         <v>49</v>
       </c>
       <c r="D236" s="21" t="s">
+        <v>517</v>
+      </c>
+      <c r="E236" s="22" t="s">
         <v>518</v>
-      </c>
-      <c r="E236" s="22" t="s">
-        <v>519</v>
       </c>
       <c r="F236" s="23"/>
       <c r="G236" s="24"/>
@@ -15295,10 +15306,10 @@
         <v>49</v>
       </c>
       <c r="D237" s="21" t="s">
+        <v>519</v>
+      </c>
+      <c r="E237" s="22" t="s">
         <v>520</v>
-      </c>
-      <c r="E237" s="22" t="s">
-        <v>521</v>
       </c>
       <c r="F237" s="23"/>
       <c r="G237" s="24"/>
@@ -15329,10 +15340,10 @@
         <v>49</v>
       </c>
       <c r="D238" s="21" t="s">
+        <v>521</v>
+      </c>
+      <c r="E238" s="22" t="s">
         <v>522</v>
-      </c>
-      <c r="E238" s="22" t="s">
-        <v>523</v>
       </c>
       <c r="F238" s="23"/>
       <c r="G238" s="24"/>
@@ -15363,10 +15374,10 @@
         <v>49</v>
       </c>
       <c r="D239" s="21" t="s">
+        <v>523</v>
+      </c>
+      <c r="E239" s="22" t="s">
         <v>524</v>
-      </c>
-      <c r="E239" s="22" t="s">
-        <v>525</v>
       </c>
       <c r="F239" s="23"/>
       <c r="G239" s="24"/>
@@ -15397,10 +15408,10 @@
         <v>49</v>
       </c>
       <c r="D240" s="21" t="s">
+        <v>525</v>
+      </c>
+      <c r="E240" s="22" t="s">
         <v>526</v>
-      </c>
-      <c r="E240" s="22" t="s">
-        <v>527</v>
       </c>
       <c r="F240" s="23"/>
       <c r="G240" s="24"/>
@@ -15431,10 +15442,10 @@
         <v>49</v>
       </c>
       <c r="D241" s="21" t="s">
+        <v>527</v>
+      </c>
+      <c r="E241" s="22" t="s">
         <v>528</v>
-      </c>
-      <c r="E241" s="22" t="s">
-        <v>529</v>
       </c>
       <c r="F241" s="23"/>
       <c r="G241" s="24"/>
@@ -15465,10 +15476,10 @@
         <v>49</v>
       </c>
       <c r="D242" s="21" t="s">
+        <v>529</v>
+      </c>
+      <c r="E242" s="22" t="s">
         <v>530</v>
-      </c>
-      <c r="E242" s="22" t="s">
-        <v>531</v>
       </c>
       <c r="F242" s="23"/>
       <c r="G242" s="24"/>
@@ -15499,10 +15510,10 @@
         <v>49</v>
       </c>
       <c r="D243" s="21" t="s">
+        <v>531</v>
+      </c>
+      <c r="E243" s="22" t="s">
         <v>532</v>
-      </c>
-      <c r="E243" s="22" t="s">
-        <v>533</v>
       </c>
       <c r="F243" s="23"/>
       <c r="G243" s="24"/>
@@ -15533,10 +15544,10 @@
         <v>49</v>
       </c>
       <c r="D244" s="21" t="s">
+        <v>533</v>
+      </c>
+      <c r="E244" s="22" t="s">
         <v>534</v>
-      </c>
-      <c r="E244" s="22" t="s">
-        <v>535</v>
       </c>
       <c r="F244" s="23"/>
       <c r="G244" s="24"/>
@@ -15567,10 +15578,10 @@
         <v>49</v>
       </c>
       <c r="D245" s="21" t="s">
+        <v>535</v>
+      </c>
+      <c r="E245" s="22" t="s">
         <v>536</v>
-      </c>
-      <c r="E245" s="22" t="s">
-        <v>537</v>
       </c>
       <c r="F245" s="23"/>
       <c r="G245" s="24"/>
@@ -15601,10 +15612,10 @@
         <v>403</v>
       </c>
       <c r="D246" s="21" t="s">
+        <v>537</v>
+      </c>
+      <c r="E246" s="22" t="s">
         <v>538</v>
-      </c>
-      <c r="E246" s="22" t="s">
-        <v>539</v>
       </c>
       <c r="F246" s="23"/>
       <c r="G246" s="24"/>
@@ -15635,10 +15646,10 @@
         <v>403</v>
       </c>
       <c r="D247" s="21" t="s">
+        <v>539</v>
+      </c>
+      <c r="E247" s="22" t="s">
         <v>540</v>
-      </c>
-      <c r="E247" s="22" t="s">
-        <v>541</v>
       </c>
       <c r="F247" s="23"/>
       <c r="G247" s="24"/>
@@ -15669,10 +15680,10 @@
         <v>403</v>
       </c>
       <c r="D248" s="21" t="s">
+        <v>541</v>
+      </c>
+      <c r="E248" s="22" t="s">
         <v>542</v>
-      </c>
-      <c r="E248" s="22" t="s">
-        <v>543</v>
       </c>
       <c r="F248" s="23"/>
       <c r="G248" s="24"/>
@@ -15703,10 +15714,10 @@
         <v>403</v>
       </c>
       <c r="D249" s="21" t="s">
+        <v>543</v>
+      </c>
+      <c r="E249" s="22" t="s">
         <v>544</v>
-      </c>
-      <c r="E249" s="22" t="s">
-        <v>545</v>
       </c>
       <c r="F249" s="23"/>
       <c r="G249" s="24"/>
@@ -15737,10 +15748,10 @@
         <v>403</v>
       </c>
       <c r="D250" s="21" t="s">
+        <v>545</v>
+      </c>
+      <c r="E250" s="22" t="s">
         <v>546</v>
-      </c>
-      <c r="E250" s="22" t="s">
-        <v>547</v>
       </c>
       <c r="F250" s="23"/>
       <c r="G250" s="24"/>
@@ -15771,10 +15782,10 @@
         <v>403</v>
       </c>
       <c r="D251" s="21" t="s">
+        <v>547</v>
+      </c>
+      <c r="E251" s="22" t="s">
         <v>548</v>
-      </c>
-      <c r="E251" s="22" t="s">
-        <v>549</v>
       </c>
       <c r="F251" s="23"/>
       <c r="G251" s="24"/>
@@ -15805,10 +15816,10 @@
         <v>403</v>
       </c>
       <c r="D252" s="21" t="s">
+        <v>549</v>
+      </c>
+      <c r="E252" s="22" t="s">
         <v>550</v>
-      </c>
-      <c r="E252" s="22" t="s">
-        <v>551</v>
       </c>
       <c r="F252" s="23"/>
       <c r="G252" s="24"/>
@@ -15839,10 +15850,10 @@
         <v>403</v>
       </c>
       <c r="D253" s="21" t="s">
+        <v>551</v>
+      </c>
+      <c r="E253" s="22" t="s">
         <v>552</v>
-      </c>
-      <c r="E253" s="22" t="s">
-        <v>553</v>
       </c>
       <c r="F253" s="23"/>
       <c r="G253" s="24"/>
@@ -15873,10 +15884,10 @@
         <v>403</v>
       </c>
       <c r="D254" s="21" t="s">
+        <v>553</v>
+      </c>
+      <c r="E254" s="22" t="s">
         <v>554</v>
-      </c>
-      <c r="E254" s="22" t="s">
-        <v>555</v>
       </c>
       <c r="F254" s="23"/>
       <c r="G254" s="24"/>
@@ -15907,7 +15918,7 @@
         <v>403</v>
       </c>
       <c r="D255" s="21" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E255" s="22" t="s">
         <v>291</v>
@@ -15941,7 +15952,7 @@
         <v>403</v>
       </c>
       <c r="D256" s="21" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E256" s="22" t="s">
         <v>294</v>
@@ -15975,7 +15986,7 @@
         <v>403</v>
       </c>
       <c r="D257" s="21" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E257" s="22" t="s">
         <v>300</v>
@@ -16011,10 +16022,10 @@
         <v>61</v>
       </c>
       <c r="D258" s="21" t="s">
+        <v>558</v>
+      </c>
+      <c r="E258" s="22" t="s">
         <v>559</v>
-      </c>
-      <c r="E258" s="22" t="s">
-        <v>560</v>
       </c>
       <c r="F258" s="23"/>
       <c r="G258" s="24"/>
@@ -16045,10 +16056,10 @@
         <v>61</v>
       </c>
       <c r="D259" s="21" t="s">
+        <v>560</v>
+      </c>
+      <c r="E259" s="22" t="s">
         <v>561</v>
-      </c>
-      <c r="E259" s="22" t="s">
-        <v>562</v>
       </c>
       <c r="F259" s="23"/>
       <c r="G259" s="24"/>
@@ -16079,10 +16090,10 @@
         <v>61</v>
       </c>
       <c r="D260" s="21" t="s">
+        <v>562</v>
+      </c>
+      <c r="E260" s="22" t="s">
         <v>563</v>
-      </c>
-      <c r="E260" s="22" t="s">
-        <v>564</v>
       </c>
       <c r="F260" s="23"/>
       <c r="G260" s="24"/>
@@ -16113,10 +16124,10 @@
         <v>61</v>
       </c>
       <c r="D261" s="21" t="s">
+        <v>564</v>
+      </c>
+      <c r="E261" s="22" t="s">
         <v>565</v>
-      </c>
-      <c r="E261" s="22" t="s">
-        <v>566</v>
       </c>
       <c r="F261" s="23"/>
       <c r="G261" s="24"/>
@@ -16147,10 +16158,10 @@
         <v>61</v>
       </c>
       <c r="D262" s="21" t="s">
+        <v>566</v>
+      </c>
+      <c r="E262" s="22" t="s">
         <v>567</v>
-      </c>
-      <c r="E262" s="22" t="s">
-        <v>568</v>
       </c>
       <c r="F262" s="23"/>
       <c r="G262" s="24"/>
@@ -16181,10 +16192,10 @@
         <v>61</v>
       </c>
       <c r="D263" s="21" t="s">
+        <v>568</v>
+      </c>
+      <c r="E263" s="22" t="s">
         <v>569</v>
-      </c>
-      <c r="E263" s="22" t="s">
-        <v>570</v>
       </c>
       <c r="F263" s="23"/>
       <c r="G263" s="24"/>
@@ -16215,10 +16226,10 @@
         <v>61</v>
       </c>
       <c r="D264" s="21" t="s">
+        <v>570</v>
+      </c>
+      <c r="E264" s="22" t="s">
         <v>571</v>
-      </c>
-      <c r="E264" s="22" t="s">
-        <v>572</v>
       </c>
       <c r="F264" s="23"/>
       <c r="G264" s="24"/>
@@ -16249,10 +16260,10 @@
         <v>61</v>
       </c>
       <c r="D265" s="21" t="s">
+        <v>572</v>
+      </c>
+      <c r="E265" s="22" t="s">
         <v>573</v>
-      </c>
-      <c r="E265" s="22" t="s">
-        <v>574</v>
       </c>
       <c r="F265" s="23"/>
       <c r="G265" s="24"/>
@@ -16283,10 +16294,10 @@
         <v>61</v>
       </c>
       <c r="D266" s="21" t="s">
+        <v>574</v>
+      </c>
+      <c r="E266" s="22" t="s">
         <v>575</v>
-      </c>
-      <c r="E266" s="22" t="s">
-        <v>576</v>
       </c>
       <c r="F266" s="23"/>
       <c r="G266" s="24"/>
@@ -16317,10 +16328,10 @@
         <v>61</v>
       </c>
       <c r="D267" s="21" t="s">
+        <v>576</v>
+      </c>
+      <c r="E267" s="22" t="s">
         <v>577</v>
-      </c>
-      <c r="E267" s="22" t="s">
-        <v>578</v>
       </c>
       <c r="F267" s="23"/>
       <c r="G267" s="24"/>
@@ -16351,10 +16362,10 @@
         <v>61</v>
       </c>
       <c r="D268" s="21" t="s">
+        <v>578</v>
+      </c>
+      <c r="E268" s="22" t="s">
         <v>579</v>
-      </c>
-      <c r="E268" s="22" t="s">
-        <v>580</v>
       </c>
       <c r="F268" s="23"/>
       <c r="G268" s="24"/>
@@ -16385,10 +16396,10 @@
         <v>61</v>
       </c>
       <c r="D269" s="21" t="s">
+        <v>580</v>
+      </c>
+      <c r="E269" s="22" t="s">
         <v>581</v>
-      </c>
-      <c r="E269" s="22" t="s">
-        <v>582</v>
       </c>
       <c r="F269" s="23"/>
       <c r="G269" s="24"/>
@@ -16419,10 +16430,10 @@
         <v>61</v>
       </c>
       <c r="D270" s="21" t="s">
+        <v>582</v>
+      </c>
+      <c r="E270" s="22" t="s">
         <v>583</v>
-      </c>
-      <c r="E270" s="22" t="s">
-        <v>584</v>
       </c>
       <c r="F270" s="23"/>
       <c r="G270" s="24"/>
@@ -16453,10 +16464,10 @@
         <v>61</v>
       </c>
       <c r="D271" s="21" t="s">
+        <v>584</v>
+      </c>
+      <c r="E271" s="22" t="s">
         <v>585</v>
-      </c>
-      <c r="E271" s="22" t="s">
-        <v>586</v>
       </c>
       <c r="F271" s="23"/>
       <c r="G271" s="24"/>
@@ -16487,10 +16498,10 @@
         <v>61</v>
       </c>
       <c r="D272" s="21" t="s">
+        <v>586</v>
+      </c>
+      <c r="E272" s="22" t="s">
         <v>587</v>
-      </c>
-      <c r="E272" s="22" t="s">
-        <v>588</v>
       </c>
       <c r="F272" s="23"/>
       <c r="G272" s="24"/>
@@ -16521,10 +16532,10 @@
         <v>61</v>
       </c>
       <c r="D273" s="21" t="s">
+        <v>588</v>
+      </c>
+      <c r="E273" s="22" t="s">
         <v>589</v>
-      </c>
-      <c r="E273" s="22" t="s">
-        <v>590</v>
       </c>
       <c r="F273" s="23"/>
       <c r="G273" s="24"/>
@@ -16555,10 +16566,10 @@
         <v>61</v>
       </c>
       <c r="D274" s="21" t="s">
+        <v>590</v>
+      </c>
+      <c r="E274" s="22" t="s">
         <v>591</v>
-      </c>
-      <c r="E274" s="22" t="s">
-        <v>592</v>
       </c>
       <c r="F274" s="23"/>
       <c r="G274" s="24"/>
@@ -16589,10 +16600,10 @@
         <v>61</v>
       </c>
       <c r="D275" s="21" t="s">
+        <v>592</v>
+      </c>
+      <c r="E275" s="22" t="s">
         <v>593</v>
-      </c>
-      <c r="E275" s="22" t="s">
-        <v>594</v>
       </c>
       <c r="F275" s="23"/>
       <c r="G275" s="24"/>
@@ -16623,10 +16634,10 @@
         <v>61</v>
       </c>
       <c r="D276" s="21" t="s">
+        <v>594</v>
+      </c>
+      <c r="E276" s="22" t="s">
         <v>595</v>
-      </c>
-      <c r="E276" s="22" t="s">
-        <v>596</v>
       </c>
       <c r="F276" s="23"/>
       <c r="G276" s="24"/>
@@ -16657,10 +16668,10 @@
         <v>66</v>
       </c>
       <c r="D277" s="21" t="s">
+        <v>596</v>
+      </c>
+      <c r="E277" s="22" t="s">
         <v>597</v>
-      </c>
-      <c r="E277" s="22" t="s">
-        <v>598</v>
       </c>
       <c r="F277" s="23"/>
       <c r="G277" s="24"/>
@@ -16691,10 +16702,10 @@
         <v>66</v>
       </c>
       <c r="D278" s="21" t="s">
+        <v>598</v>
+      </c>
+      <c r="E278" s="22" t="s">
         <v>599</v>
-      </c>
-      <c r="E278" s="22" t="s">
-        <v>600</v>
       </c>
       <c r="F278" s="23"/>
       <c r="G278" s="24"/>
@@ -16725,10 +16736,10 @@
         <v>66</v>
       </c>
       <c r="D279" s="21" t="s">
+        <v>600</v>
+      </c>
+      <c r="E279" s="22" t="s">
         <v>601</v>
-      </c>
-      <c r="E279" s="22" t="s">
-        <v>602</v>
       </c>
       <c r="F279" s="23"/>
       <c r="G279" s="24"/>
@@ -16759,10 +16770,10 @@
         <v>66</v>
       </c>
       <c r="D280" s="21" t="s">
+        <v>602</v>
+      </c>
+      <c r="E280" s="22" t="s">
         <v>603</v>
-      </c>
-      <c r="E280" s="22" t="s">
-        <v>604</v>
       </c>
       <c r="F280" s="23"/>
       <c r="G280" s="24"/>
@@ -16793,10 +16804,10 @@
         <v>66</v>
       </c>
       <c r="D281" s="21" t="s">
+        <v>604</v>
+      </c>
+      <c r="E281" s="22" t="s">
         <v>605</v>
-      </c>
-      <c r="E281" s="22" t="s">
-        <v>606</v>
       </c>
       <c r="F281" s="23"/>
       <c r="G281" s="24"/>
@@ -16827,10 +16838,10 @@
         <v>66</v>
       </c>
       <c r="D282" s="21" t="s">
+        <v>606</v>
+      </c>
+      <c r="E282" s="22" t="s">
         <v>607</v>
-      </c>
-      <c r="E282" s="22" t="s">
-        <v>608</v>
       </c>
       <c r="F282" s="23"/>
       <c r="G282" s="24"/>
@@ -16861,10 +16872,10 @@
         <v>66</v>
       </c>
       <c r="D283" s="21" t="s">
+        <v>608</v>
+      </c>
+      <c r="E283" s="22" t="s">
         <v>609</v>
-      </c>
-      <c r="E283" s="22" t="s">
-        <v>610</v>
       </c>
       <c r="F283" s="23"/>
       <c r="G283" s="24"/>
@@ -16895,10 +16906,10 @@
         <v>66</v>
       </c>
       <c r="D284" s="21" t="s">
+        <v>610</v>
+      </c>
+      <c r="E284" s="22" t="s">
         <v>611</v>
-      </c>
-      <c r="E284" s="22" t="s">
-        <v>612</v>
       </c>
       <c r="F284" s="23"/>
       <c r="G284" s="24"/>
@@ -16929,10 +16940,10 @@
         <v>66</v>
       </c>
       <c r="D285" s="21" t="s">
+        <v>612</v>
+      </c>
+      <c r="E285" s="22" t="s">
         <v>613</v>
-      </c>
-      <c r="E285" s="22" t="s">
-        <v>614</v>
       </c>
       <c r="F285" s="23"/>
       <c r="G285" s="24"/>
@@ -16963,10 +16974,10 @@
         <v>66</v>
       </c>
       <c r="D286" s="21" t="s">
+        <v>614</v>
+      </c>
+      <c r="E286" s="22" t="s">
         <v>615</v>
-      </c>
-      <c r="E286" s="22" t="s">
-        <v>616</v>
       </c>
       <c r="F286" s="23"/>
       <c r="G286" s="24"/>
@@ -16997,10 +17008,10 @@
         <v>66</v>
       </c>
       <c r="D287" s="21" t="s">
+        <v>616</v>
+      </c>
+      <c r="E287" s="22" t="s">
         <v>617</v>
-      </c>
-      <c r="E287" s="22" t="s">
-        <v>618</v>
       </c>
       <c r="F287" s="23"/>
       <c r="G287" s="24"/>
@@ -17031,10 +17042,10 @@
         <v>66</v>
       </c>
       <c r="D288" s="21" t="s">
+        <v>618</v>
+      </c>
+      <c r="E288" s="22" t="s">
         <v>619</v>
-      </c>
-      <c r="E288" s="22" t="s">
-        <v>620</v>
       </c>
       <c r="F288" s="23"/>
       <c r="G288" s="24"/>
@@ -17065,10 +17076,10 @@
         <v>66</v>
       </c>
       <c r="D289" s="21" t="s">
+        <v>620</v>
+      </c>
+      <c r="E289" s="22" t="s">
         <v>621</v>
-      </c>
-      <c r="E289" s="22" t="s">
-        <v>622</v>
       </c>
       <c r="F289" s="23"/>
       <c r="G289" s="24"/>
@@ -17099,10 +17110,10 @@
         <v>71</v>
       </c>
       <c r="D290" s="21" t="s">
+        <v>622</v>
+      </c>
+      <c r="E290" s="22" t="s">
         <v>623</v>
-      </c>
-      <c r="E290" s="22" t="s">
-        <v>624</v>
       </c>
       <c r="F290" s="23"/>
       <c r="G290" s="24"/>
@@ -17133,10 +17144,10 @@
         <v>71</v>
       </c>
       <c r="D291" s="21" t="s">
+        <v>624</v>
+      </c>
+      <c r="E291" s="22" t="s">
         <v>625</v>
-      </c>
-      <c r="E291" s="22" t="s">
-        <v>626</v>
       </c>
       <c r="F291" s="23"/>
       <c r="G291" s="24"/>
@@ -17167,10 +17178,10 @@
         <v>71</v>
       </c>
       <c r="D292" s="21" t="s">
+        <v>626</v>
+      </c>
+      <c r="E292" s="22" t="s">
         <v>627</v>
-      </c>
-      <c r="E292" s="22" t="s">
-        <v>628</v>
       </c>
       <c r="F292" s="23"/>
       <c r="G292" s="24"/>
@@ -17201,10 +17212,10 @@
         <v>71</v>
       </c>
       <c r="D293" s="21" t="s">
+        <v>628</v>
+      </c>
+      <c r="E293" s="22" t="s">
         <v>629</v>
-      </c>
-      <c r="E293" s="22" t="s">
-        <v>630</v>
       </c>
       <c r="F293" s="23"/>
       <c r="G293" s="24"/>
@@ -17235,10 +17246,10 @@
         <v>71</v>
       </c>
       <c r="D294" s="21" t="s">
+        <v>630</v>
+      </c>
+      <c r="E294" s="22" t="s">
         <v>631</v>
-      </c>
-      <c r="E294" s="22" t="s">
-        <v>632</v>
       </c>
       <c r="F294" s="23"/>
       <c r="G294" s="24"/>
@@ -17269,10 +17280,10 @@
         <v>71</v>
       </c>
       <c r="D295" s="21" t="s">
+        <v>632</v>
+      </c>
+      <c r="E295" s="22" t="s">
         <v>633</v>
-      </c>
-      <c r="E295" s="22" t="s">
-        <v>634</v>
       </c>
       <c r="F295" s="23"/>
       <c r="G295" s="24"/>
@@ -17303,10 +17314,10 @@
         <v>71</v>
       </c>
       <c r="D296" s="21" t="s">
+        <v>634</v>
+      </c>
+      <c r="E296" s="22" t="s">
         <v>635</v>
-      </c>
-      <c r="E296" s="22" t="s">
-        <v>636</v>
       </c>
       <c r="F296" s="23"/>
       <c r="G296" s="24"/>
@@ -17337,10 +17348,10 @@
         <v>71</v>
       </c>
       <c r="D297" s="21" t="s">
+        <v>636</v>
+      </c>
+      <c r="E297" s="22" t="s">
         <v>637</v>
-      </c>
-      <c r="E297" s="22" t="s">
-        <v>638</v>
       </c>
       <c r="F297" s="23"/>
       <c r="G297" s="24"/>
@@ -17371,10 +17382,10 @@
         <v>71</v>
       </c>
       <c r="D298" s="21" t="s">
+        <v>638</v>
+      </c>
+      <c r="E298" s="22" t="s">
         <v>639</v>
-      </c>
-      <c r="E298" s="22" t="s">
-        <v>640</v>
       </c>
       <c r="F298" s="23"/>
       <c r="G298" s="24"/>
@@ -17405,10 +17416,10 @@
         <v>71</v>
       </c>
       <c r="D299" s="21" t="s">
+        <v>640</v>
+      </c>
+      <c r="E299" s="22" t="s">
         <v>641</v>
-      </c>
-      <c r="E299" s="22" t="s">
-        <v>642</v>
       </c>
       <c r="F299" s="23"/>
       <c r="G299" s="24"/>
@@ -17439,10 +17450,10 @@
         <v>71</v>
       </c>
       <c r="D300" s="21" t="s">
+        <v>642</v>
+      </c>
+      <c r="E300" s="22" t="s">
         <v>643</v>
-      </c>
-      <c r="E300" s="22" t="s">
-        <v>644</v>
       </c>
       <c r="F300" s="23"/>
       <c r="G300" s="24"/>
@@ -17473,10 +17484,10 @@
         <v>71</v>
       </c>
       <c r="D301" s="21" t="s">
+        <v>644</v>
+      </c>
+      <c r="E301" s="22" t="s">
         <v>645</v>
-      </c>
-      <c r="E301" s="22" t="s">
-        <v>646</v>
       </c>
       <c r="F301" s="23"/>
       <c r="G301" s="24"/>
@@ -17507,10 +17518,10 @@
         <v>71</v>
       </c>
       <c r="D302" s="21" t="s">
+        <v>646</v>
+      </c>
+      <c r="E302" s="22" t="s">
         <v>647</v>
-      </c>
-      <c r="E302" s="22" t="s">
-        <v>648</v>
       </c>
       <c r="F302" s="23"/>
       <c r="G302" s="24"/>
@@ -17541,10 +17552,10 @@
         <v>71</v>
       </c>
       <c r="D303" s="21" t="s">
+        <v>648</v>
+      </c>
+      <c r="E303" s="22" t="s">
         <v>649</v>
-      </c>
-      <c r="E303" s="22" t="s">
-        <v>650</v>
       </c>
       <c r="F303" s="23"/>
       <c r="G303" s="24"/>
@@ -17575,10 +17586,10 @@
         <v>71</v>
       </c>
       <c r="D304" s="21" t="s">
+        <v>650</v>
+      </c>
+      <c r="E304" s="22" t="s">
         <v>651</v>
-      </c>
-      <c r="E304" s="22" t="s">
-        <v>652</v>
       </c>
       <c r="F304" s="23"/>
       <c r="G304" s="24"/>
@@ -17609,10 +17620,10 @@
         <v>76</v>
       </c>
       <c r="D305" s="38" t="s">
+        <v>652</v>
+      </c>
+      <c r="E305" s="39" t="s">
         <v>653</v>
-      </c>
-      <c r="E305" s="39" t="s">
-        <v>654</v>
       </c>
       <c r="F305" s="40"/>
       <c r="G305" s="41"/>
@@ -17622,7 +17633,7 @@
         <v>218</v>
       </c>
       <c r="K305" s="33" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="L305" s="33"/>
       <c r="M305" s="33"/>
@@ -17647,10 +17658,10 @@
         <v>76</v>
       </c>
       <c r="D306" s="38" t="s">
+        <v>655</v>
+      </c>
+      <c r="E306" s="39" t="s">
         <v>656</v>
-      </c>
-      <c r="E306" s="39" t="s">
-        <v>657</v>
       </c>
       <c r="F306" s="40"/>
       <c r="G306" s="41"/>
@@ -17660,7 +17671,7 @@
         <v>218</v>
       </c>
       <c r="K306" s="33" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="L306" s="33"/>
       <c r="M306" s="33"/>
@@ -17685,10 +17696,10 @@
         <v>76</v>
       </c>
       <c r="D307" s="38" t="s">
+        <v>658</v>
+      </c>
+      <c r="E307" s="39" t="s">
         <v>659</v>
-      </c>
-      <c r="E307" s="39" t="s">
-        <v>660</v>
       </c>
       <c r="F307" s="40"/>
       <c r="G307" s="41"/>
@@ -17698,7 +17709,7 @@
         <v>218</v>
       </c>
       <c r="K307" s="33" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="L307" s="33"/>
       <c r="M307" s="33"/>
@@ -17723,10 +17734,10 @@
         <v>76</v>
       </c>
       <c r="D308" s="38" t="s">
+        <v>661</v>
+      </c>
+      <c r="E308" s="39" t="s">
         <v>662</v>
-      </c>
-      <c r="E308" s="39" t="s">
-        <v>663</v>
       </c>
       <c r="F308" s="40"/>
       <c r="G308" s="41"/>
@@ -17736,7 +17747,7 @@
         <v>218</v>
       </c>
       <c r="K308" s="33" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="L308" s="33"/>
       <c r="M308" s="33"/>
@@ -17761,10 +17772,10 @@
         <v>76</v>
       </c>
       <c r="D309" s="38" t="s">
+        <v>664</v>
+      </c>
+      <c r="E309" s="39" t="s">
         <v>665</v>
-      </c>
-      <c r="E309" s="39" t="s">
-        <v>666</v>
       </c>
       <c r="F309" s="40"/>
       <c r="G309" s="41"/>
@@ -17799,10 +17810,10 @@
         <v>76</v>
       </c>
       <c r="D310" s="38" t="s">
+        <v>666</v>
+      </c>
+      <c r="E310" s="39" t="s">
         <v>667</v>
-      </c>
-      <c r="E310" s="39" t="s">
-        <v>668</v>
       </c>
       <c r="F310" s="40"/>
       <c r="G310" s="41"/>
@@ -17837,10 +17848,10 @@
         <v>76</v>
       </c>
       <c r="D311" s="38" t="s">
+        <v>668</v>
+      </c>
+      <c r="E311" s="39" t="s">
         <v>669</v>
-      </c>
-      <c r="E311" s="39" t="s">
-        <v>670</v>
       </c>
       <c r="F311" s="40"/>
       <c r="G311" s="41"/>
@@ -17850,7 +17861,7 @@
         <v>218</v>
       </c>
       <c r="K311" s="33" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="L311" s="33"/>
       <c r="M311" s="33"/>
@@ -17875,10 +17886,10 @@
         <v>76</v>
       </c>
       <c r="D312" s="38" t="s">
+        <v>671</v>
+      </c>
+      <c r="E312" s="39" t="s">
         <v>672</v>
-      </c>
-      <c r="E312" s="39" t="s">
-        <v>673</v>
       </c>
       <c r="F312" s="40"/>
       <c r="G312" s="41"/>
@@ -17888,7 +17899,7 @@
         <v>218</v>
       </c>
       <c r="K312" s="33" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="L312" s="33"/>
       <c r="M312" s="33"/>
@@ -17913,10 +17924,10 @@
         <v>76</v>
       </c>
       <c r="D313" s="38" t="s">
+        <v>674</v>
+      </c>
+      <c r="E313" s="39" t="s">
         <v>675</v>
-      </c>
-      <c r="E313" s="39" t="s">
-        <v>676</v>
       </c>
       <c r="F313" s="40"/>
       <c r="G313" s="41"/>
@@ -17926,7 +17937,7 @@
         <v>218</v>
       </c>
       <c r="K313" s="33" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="L313" s="33"/>
       <c r="M313" s="33"/>
@@ -17951,10 +17962,10 @@
         <v>76</v>
       </c>
       <c r="D314" s="38" t="s">
+        <v>677</v>
+      </c>
+      <c r="E314" s="39" t="s">
         <v>678</v>
-      </c>
-      <c r="E314" s="39" t="s">
-        <v>679</v>
       </c>
       <c r="F314" s="40"/>
       <c r="G314" s="41"/>
@@ -17964,7 +17975,7 @@
         <v>218</v>
       </c>
       <c r="K314" s="33" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="L314" s="33"/>
       <c r="M314" s="33"/>
@@ -17989,10 +18000,10 @@
         <v>76</v>
       </c>
       <c r="D315" s="38" t="s">
+        <v>680</v>
+      </c>
+      <c r="E315" s="39" t="s">
         <v>681</v>
-      </c>
-      <c r="E315" s="39" t="s">
-        <v>682</v>
       </c>
       <c r="F315" s="40"/>
       <c r="G315" s="41"/>
@@ -18002,7 +18013,7 @@
         <v>218</v>
       </c>
       <c r="K315" s="33" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="L315" s="33"/>
       <c r="M315" s="33"/>
@@ -18027,10 +18038,10 @@
         <v>76</v>
       </c>
       <c r="D316" s="38" t="s">
+        <v>683</v>
+      </c>
+      <c r="E316" s="39" t="s">
         <v>684</v>
-      </c>
-      <c r="E316" s="39" t="s">
-        <v>685</v>
       </c>
       <c r="F316" s="40"/>
       <c r="G316" s="41"/>
@@ -18040,7 +18051,7 @@
         <v>218</v>
       </c>
       <c r="K316" s="33" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="L316" s="33"/>
       <c r="M316" s="33"/>
@@ -18065,10 +18076,10 @@
         <v>76</v>
       </c>
       <c r="D317" s="38" t="s">
+        <v>686</v>
+      </c>
+      <c r="E317" s="39" t="s">
         <v>687</v>
-      </c>
-      <c r="E317" s="39" t="s">
-        <v>688</v>
       </c>
       <c r="F317" s="40"/>
       <c r="G317" s="41"/>
@@ -18078,7 +18089,7 @@
         <v>218</v>
       </c>
       <c r="K317" s="33" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L317" s="33"/>
       <c r="M317" s="33"/>
@@ -18103,10 +18114,10 @@
         <v>76</v>
       </c>
       <c r="D318" s="38" t="s">
+        <v>688</v>
+      </c>
+      <c r="E318" s="39" t="s">
         <v>689</v>
-      </c>
-      <c r="E318" s="39" t="s">
-        <v>690</v>
       </c>
       <c r="F318" s="40"/>
       <c r="G318" s="41"/>
@@ -18116,7 +18127,7 @@
         <v>218</v>
       </c>
       <c r="K318" s="33" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L318" s="33"/>
       <c r="M318" s="33"/>
@@ -18141,10 +18152,10 @@
         <v>76</v>
       </c>
       <c r="D319" s="38" t="s">
+        <v>690</v>
+      </c>
+      <c r="E319" s="39" t="s">
         <v>691</v>
-      </c>
-      <c r="E319" s="39" t="s">
-        <v>692</v>
       </c>
       <c r="F319" s="40"/>
       <c r="G319" s="41"/>
@@ -18154,7 +18165,7 @@
         <v>218</v>
       </c>
       <c r="K319" s="33" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L319" s="33"/>
       <c r="M319" s="33"/>
@@ -18179,10 +18190,10 @@
         <v>76</v>
       </c>
       <c r="D320" s="38" t="s">
+        <v>692</v>
+      </c>
+      <c r="E320" s="39" t="s">
         <v>693</v>
-      </c>
-      <c r="E320" s="39" t="s">
-        <v>694</v>
       </c>
       <c r="F320" s="40"/>
       <c r="G320" s="41"/>
@@ -18192,7 +18203,7 @@
         <v>218</v>
       </c>
       <c r="K320" s="33" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L320" s="33"/>
       <c r="M320" s="33"/>
@@ -18217,10 +18228,10 @@
         <v>76</v>
       </c>
       <c r="D321" s="38" t="s">
+        <v>694</v>
+      </c>
+      <c r="E321" s="39" t="s">
         <v>695</v>
-      </c>
-      <c r="E321" s="39" t="s">
-        <v>696</v>
       </c>
       <c r="F321" s="40"/>
       <c r="G321" s="41"/>
@@ -18230,7 +18241,7 @@
         <v>218</v>
       </c>
       <c r="K321" s="33" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L321" s="33"/>
       <c r="M321" s="33"/>
@@ -18255,10 +18266,10 @@
         <v>76</v>
       </c>
       <c r="D322" s="38" t="s">
+        <v>696</v>
+      </c>
+      <c r="E322" s="39" t="s">
         <v>697</v>
-      </c>
-      <c r="E322" s="39" t="s">
-        <v>698</v>
       </c>
       <c r="F322" s="40"/>
       <c r="G322" s="41"/>
@@ -18268,7 +18279,7 @@
         <v>218</v>
       </c>
       <c r="K322" s="33" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="L322" s="33"/>
       <c r="M322" s="33"/>
@@ -18293,10 +18304,10 @@
         <v>76</v>
       </c>
       <c r="D323" s="38" t="s">
+        <v>699</v>
+      </c>
+      <c r="E323" s="39" t="s">
         <v>700</v>
-      </c>
-      <c r="E323" s="39" t="s">
-        <v>701</v>
       </c>
       <c r="F323" s="40"/>
       <c r="G323" s="41"/>
@@ -18306,7 +18317,7 @@
         <v>218</v>
       </c>
       <c r="K323" s="33" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="L323" s="33"/>
       <c r="M323" s="33"/>
@@ -18331,10 +18342,10 @@
         <v>76</v>
       </c>
       <c r="D324" s="38" t="s">
+        <v>702</v>
+      </c>
+      <c r="E324" s="39" t="s">
         <v>703</v>
-      </c>
-      <c r="E324" s="39" t="s">
-        <v>704</v>
       </c>
       <c r="F324" s="40"/>
       <c r="G324" s="41"/>
@@ -18344,7 +18355,7 @@
         <v>218</v>
       </c>
       <c r="K324" s="33" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L324" s="33"/>
       <c r="M324" s="33"/>
@@ -18369,22 +18380,22 @@
         <v>76</v>
       </c>
       <c r="D325" s="38" t="s">
+        <v>704</v>
+      </c>
+      <c r="E325" s="39" t="s">
         <v>705</v>
-      </c>
-      <c r="E325" s="39" t="s">
-        <v>706</v>
       </c>
       <c r="F325" s="40">
         <v>45002</v>
       </c>
       <c r="G325" s="41" t="s">
+        <v>706</v>
+      </c>
+      <c r="H325" s="41" t="s">
         <v>707</v>
       </c>
-      <c r="H325" s="41" t="s">
+      <c r="I325" s="41" t="s">
         <v>708</v>
-      </c>
-      <c r="I325" s="41" t="s">
-        <v>709</v>
       </c>
       <c r="J325" s="33" t="s">
         <v>215</v>
@@ -18397,7 +18408,7 @@
         <v>218</v>
       </c>
       <c r="N325" s="33" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="O325" s="33" t="s">
         <v>215</v>
@@ -18423,22 +18434,22 @@
         <v>76</v>
       </c>
       <c r="D326" s="38" t="s">
+        <v>710</v>
+      </c>
+      <c r="E326" s="39" t="s">
         <v>711</v>
-      </c>
-      <c r="E326" s="39" t="s">
-        <v>712</v>
       </c>
       <c r="F326" s="40">
         <v>45002</v>
       </c>
       <c r="G326" s="41" t="s">
+        <v>712</v>
+      </c>
+      <c r="H326" s="41" t="s">
         <v>713</v>
       </c>
-      <c r="H326" s="41" t="s">
+      <c r="I326" s="41" t="s">
         <v>714</v>
-      </c>
-      <c r="I326" s="41" t="s">
-        <v>715</v>
       </c>
       <c r="J326" s="33" t="s">
         <v>215</v>
@@ -18451,7 +18462,7 @@
         <v>218</v>
       </c>
       <c r="N326" s="33" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="O326" s="33" t="s">
         <v>215</v>
@@ -18477,10 +18488,10 @@
         <v>76</v>
       </c>
       <c r="D327" s="38" t="s">
+        <v>716</v>
+      </c>
+      <c r="E327" s="39" t="s">
         <v>717</v>
-      </c>
-      <c r="E327" s="39" t="s">
-        <v>718</v>
       </c>
       <c r="F327" s="40"/>
       <c r="G327" s="41"/>
@@ -18490,7 +18501,7 @@
         <v>218</v>
       </c>
       <c r="K327" s="33" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="L327" s="33"/>
       <c r="M327" s="33"/>
@@ -18515,10 +18526,10 @@
         <v>76</v>
       </c>
       <c r="D328" s="38" t="s">
+        <v>719</v>
+      </c>
+      <c r="E328" s="39" t="s">
         <v>720</v>
-      </c>
-      <c r="E328" s="39" t="s">
-        <v>721</v>
       </c>
       <c r="F328" s="40"/>
       <c r="G328" s="41"/>
@@ -18528,7 +18539,7 @@
         <v>218</v>
       </c>
       <c r="K328" s="33" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L328" s="33"/>
       <c r="M328" s="33"/>
@@ -18553,10 +18564,10 @@
         <v>76</v>
       </c>
       <c r="D329" s="38" t="s">
+        <v>721</v>
+      </c>
+      <c r="E329" s="39" t="s">
         <v>722</v>
-      </c>
-      <c r="E329" s="39" t="s">
-        <v>723</v>
       </c>
       <c r="F329" s="40"/>
       <c r="G329" s="41"/>
@@ -18566,7 +18577,7 @@
         <v>218</v>
       </c>
       <c r="K329" s="33" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="L329" s="33"/>
       <c r="M329" s="33"/>
@@ -18591,10 +18602,10 @@
         <v>403</v>
       </c>
       <c r="D330" s="21" t="s">
+        <v>723</v>
+      </c>
+      <c r="E330" s="22" t="s">
         <v>724</v>
-      </c>
-      <c r="E330" s="22" t="s">
-        <v>725</v>
       </c>
       <c r="F330" s="23"/>
       <c r="G330" s="24"/>
@@ -18625,10 +18636,10 @@
         <v>403</v>
       </c>
       <c r="D331" s="21" t="s">
+        <v>725</v>
+      </c>
+      <c r="E331" s="22" t="s">
         <v>726</v>
-      </c>
-      <c r="E331" s="22" t="s">
-        <v>727</v>
       </c>
       <c r="F331" s="23"/>
       <c r="G331" s="24"/>
@@ -18659,10 +18670,10 @@
         <v>403</v>
       </c>
       <c r="D332" s="21" t="s">
+        <v>727</v>
+      </c>
+      <c r="E332" s="22" t="s">
         <v>728</v>
-      </c>
-      <c r="E332" s="22" t="s">
-        <v>729</v>
       </c>
       <c r="F332" s="23"/>
       <c r="G332" s="24"/>
@@ -18693,10 +18704,10 @@
         <v>403</v>
       </c>
       <c r="D333" s="21" t="s">
+        <v>729</v>
+      </c>
+      <c r="E333" s="22" t="s">
         <v>730</v>
-      </c>
-      <c r="E333" s="22" t="s">
-        <v>731</v>
       </c>
       <c r="F333" s="23"/>
       <c r="G333" s="24"/>
@@ -18727,10 +18738,10 @@
         <v>403</v>
       </c>
       <c r="D334" s="21" t="s">
+        <v>731</v>
+      </c>
+      <c r="E334" s="22" t="s">
         <v>732</v>
-      </c>
-      <c r="E334" s="22" t="s">
-        <v>733</v>
       </c>
       <c r="F334" s="23"/>
       <c r="G334" s="24"/>
@@ -18761,10 +18772,10 @@
         <v>403</v>
       </c>
       <c r="D335" s="21" t="s">
+        <v>733</v>
+      </c>
+      <c r="E335" s="22" t="s">
         <v>734</v>
-      </c>
-      <c r="E335" s="22" t="s">
-        <v>735</v>
       </c>
       <c r="F335" s="23"/>
       <c r="G335" s="24"/>
@@ -18795,10 +18806,10 @@
         <v>403</v>
       </c>
       <c r="D336" s="21" t="s">
+        <v>735</v>
+      </c>
+      <c r="E336" s="22" t="s">
         <v>736</v>
-      </c>
-      <c r="E336" s="22" t="s">
-        <v>737</v>
       </c>
       <c r="F336" s="23"/>
       <c r="G336" s="24"/>
@@ -18829,10 +18840,10 @@
         <v>403</v>
       </c>
       <c r="D337" s="21" t="s">
+        <v>737</v>
+      </c>
+      <c r="E337" s="22" t="s">
         <v>738</v>
-      </c>
-      <c r="E337" s="22" t="s">
-        <v>739</v>
       </c>
       <c r="F337" s="23"/>
       <c r="G337" s="24"/>
@@ -18863,10 +18874,10 @@
         <v>403</v>
       </c>
       <c r="D338" s="21" t="s">
+        <v>739</v>
+      </c>
+      <c r="E338" s="22" t="s">
         <v>740</v>
-      </c>
-      <c r="E338" s="22" t="s">
-        <v>741</v>
       </c>
       <c r="F338" s="23"/>
       <c r="G338" s="24"/>
@@ -18897,10 +18908,10 @@
         <v>403</v>
       </c>
       <c r="D339" s="21" t="s">
+        <v>741</v>
+      </c>
+      <c r="E339" s="22" t="s">
         <v>742</v>
-      </c>
-      <c r="E339" s="22" t="s">
-        <v>743</v>
       </c>
       <c r="F339" s="23"/>
       <c r="G339" s="24"/>
@@ -18931,10 +18942,10 @@
         <v>403</v>
       </c>
       <c r="D340" s="21" t="s">
+        <v>743</v>
+      </c>
+      <c r="E340" s="22" t="s">
         <v>744</v>
-      </c>
-      <c r="E340" s="22" t="s">
-        <v>745</v>
       </c>
       <c r="F340" s="23"/>
       <c r="G340" s="24"/>
@@ -18965,10 +18976,10 @@
         <v>403</v>
       </c>
       <c r="D341" s="21" t="s">
+        <v>745</v>
+      </c>
+      <c r="E341" s="22" t="s">
         <v>746</v>
-      </c>
-      <c r="E341" s="22" t="s">
-        <v>747</v>
       </c>
       <c r="F341" s="23"/>
       <c r="G341" s="24"/>
@@ -18999,10 +19010,10 @@
         <v>403</v>
       </c>
       <c r="D342" s="21" t="s">
+        <v>747</v>
+      </c>
+      <c r="E342" s="22" t="s">
         <v>748</v>
-      </c>
-      <c r="E342" s="22" t="s">
-        <v>749</v>
       </c>
       <c r="F342" s="23"/>
       <c r="G342" s="24"/>
@@ -19033,10 +19044,10 @@
         <v>403</v>
       </c>
       <c r="D343" s="21" t="s">
+        <v>749</v>
+      </c>
+      <c r="E343" s="22" t="s">
         <v>750</v>
-      </c>
-      <c r="E343" s="22" t="s">
-        <v>751</v>
       </c>
       <c r="F343" s="23"/>
       <c r="G343" s="24"/>
@@ -19067,10 +19078,10 @@
         <v>403</v>
       </c>
       <c r="D344" s="21" t="s">
+        <v>751</v>
+      </c>
+      <c r="E344" s="22" t="s">
         <v>752</v>
-      </c>
-      <c r="E344" s="22" t="s">
-        <v>753</v>
       </c>
       <c r="F344" s="23"/>
       <c r="G344" s="24"/>
@@ -19101,10 +19112,10 @@
         <v>403</v>
       </c>
       <c r="D345" s="21" t="s">
+        <v>753</v>
+      </c>
+      <c r="E345" s="22" t="s">
         <v>754</v>
-      </c>
-      <c r="E345" s="22" t="s">
-        <v>755</v>
       </c>
       <c r="F345" s="23"/>
       <c r="G345" s="24"/>
@@ -19135,10 +19146,10 @@
         <v>403</v>
       </c>
       <c r="D346" s="21" t="s">
+        <v>755</v>
+      </c>
+      <c r="E346" s="22" t="s">
         <v>756</v>
-      </c>
-      <c r="E346" s="22" t="s">
-        <v>757</v>
       </c>
       <c r="F346" s="23"/>
       <c r="G346" s="24"/>
@@ -19169,10 +19180,10 @@
         <v>403</v>
       </c>
       <c r="D347" s="21" t="s">
+        <v>757</v>
+      </c>
+      <c r="E347" s="22" t="s">
         <v>758</v>
-      </c>
-      <c r="E347" s="22" t="s">
-        <v>759</v>
       </c>
       <c r="F347" s="23"/>
       <c r="G347" s="24"/>
@@ -19203,10 +19214,10 @@
         <v>403</v>
       </c>
       <c r="D348" s="21" t="s">
+        <v>759</v>
+      </c>
+      <c r="E348" s="22" t="s">
         <v>760</v>
-      </c>
-      <c r="E348" s="22" t="s">
-        <v>761</v>
       </c>
       <c r="F348" s="23"/>
       <c r="G348" s="24"/>
@@ -19237,10 +19248,10 @@
         <v>403</v>
       </c>
       <c r="D349" s="21" t="s">
+        <v>761</v>
+      </c>
+      <c r="E349" s="22" t="s">
         <v>762</v>
-      </c>
-      <c r="E349" s="22" t="s">
-        <v>763</v>
       </c>
       <c r="F349" s="23"/>
       <c r="G349" s="24"/>
@@ -19271,10 +19282,10 @@
         <v>403</v>
       </c>
       <c r="D350" s="21" t="s">
+        <v>763</v>
+      </c>
+      <c r="E350" s="22" t="s">
         <v>764</v>
-      </c>
-      <c r="E350" s="22" t="s">
-        <v>765</v>
       </c>
       <c r="F350" s="23"/>
       <c r="G350" s="24"/>
@@ -19305,10 +19316,10 @@
         <v>403</v>
       </c>
       <c r="D351" s="21" t="s">
+        <v>765</v>
+      </c>
+      <c r="E351" s="22" t="s">
         <v>766</v>
-      </c>
-      <c r="E351" s="22" t="s">
-        <v>767</v>
       </c>
       <c r="F351" s="23"/>
       <c r="G351" s="24"/>
@@ -19339,10 +19350,10 @@
         <v>403</v>
       </c>
       <c r="D352" s="21" t="s">
+        <v>767</v>
+      </c>
+      <c r="E352" s="22" t="s">
         <v>768</v>
-      </c>
-      <c r="E352" s="22" t="s">
-        <v>769</v>
       </c>
       <c r="F352" s="23"/>
       <c r="G352" s="24"/>
@@ -19373,10 +19384,10 @@
         <v>85</v>
       </c>
       <c r="D353" s="21" t="s">
+        <v>769</v>
+      </c>
+      <c r="E353" s="22" t="s">
         <v>770</v>
-      </c>
-      <c r="E353" s="22" t="s">
-        <v>771</v>
       </c>
       <c r="F353" s="23"/>
       <c r="G353" s="24"/>
@@ -19407,10 +19418,10 @@
         <v>85</v>
       </c>
       <c r="D354" s="21" t="s">
+        <v>771</v>
+      </c>
+      <c r="E354" s="22" t="s">
         <v>772</v>
-      </c>
-      <c r="E354" s="22" t="s">
-        <v>773</v>
       </c>
       <c r="F354" s="23"/>
       <c r="G354" s="24"/>
@@ -19441,10 +19452,10 @@
         <v>85</v>
       </c>
       <c r="D355" s="21" t="s">
+        <v>773</v>
+      </c>
+      <c r="E355" s="22" t="s">
         <v>774</v>
-      </c>
-      <c r="E355" s="22" t="s">
-        <v>775</v>
       </c>
       <c r="F355" s="23"/>
       <c r="G355" s="24"/>
@@ -19475,10 +19486,10 @@
         <v>85</v>
       </c>
       <c r="D356" s="21" t="s">
+        <v>775</v>
+      </c>
+      <c r="E356" s="22" t="s">
         <v>776</v>
-      </c>
-      <c r="E356" s="22" t="s">
-        <v>777</v>
       </c>
       <c r="F356" s="23"/>
       <c r="G356" s="24"/>
@@ -19509,10 +19520,10 @@
         <v>85</v>
       </c>
       <c r="D357" s="21" t="s">
+        <v>777</v>
+      </c>
+      <c r="E357" s="22" t="s">
         <v>778</v>
-      </c>
-      <c r="E357" s="22" t="s">
-        <v>779</v>
       </c>
       <c r="F357" s="23"/>
       <c r="G357" s="24"/>
@@ -19543,10 +19554,10 @@
         <v>85</v>
       </c>
       <c r="D358" s="21" t="s">
+        <v>779</v>
+      </c>
+      <c r="E358" s="22" t="s">
         <v>780</v>
-      </c>
-      <c r="E358" s="22" t="s">
-        <v>781</v>
       </c>
       <c r="F358" s="23"/>
       <c r="G358" s="24"/>
@@ -19577,10 +19588,10 @@
         <v>85</v>
       </c>
       <c r="D359" s="21" t="s">
+        <v>781</v>
+      </c>
+      <c r="E359" s="22" t="s">
         <v>782</v>
-      </c>
-      <c r="E359" s="22" t="s">
-        <v>783</v>
       </c>
       <c r="F359" s="23"/>
       <c r="G359" s="24"/>
@@ -19611,10 +19622,10 @@
         <v>85</v>
       </c>
       <c r="D360" s="21" t="s">
+        <v>783</v>
+      </c>
+      <c r="E360" s="22" t="s">
         <v>784</v>
-      </c>
-      <c r="E360" s="22" t="s">
-        <v>785</v>
       </c>
       <c r="F360" s="23"/>
       <c r="G360" s="24"/>
@@ -19645,10 +19656,10 @@
         <v>85</v>
       </c>
       <c r="D361" s="21" t="s">
+        <v>785</v>
+      </c>
+      <c r="E361" s="22" t="s">
         <v>786</v>
-      </c>
-      <c r="E361" s="22" t="s">
-        <v>787</v>
       </c>
       <c r="F361" s="23"/>
       <c r="G361" s="24"/>
@@ -19679,10 +19690,10 @@
         <v>85</v>
       </c>
       <c r="D362" s="21" t="s">
+        <v>787</v>
+      </c>
+      <c r="E362" s="22" t="s">
         <v>788</v>
-      </c>
-      <c r="E362" s="22" t="s">
-        <v>789</v>
       </c>
       <c r="F362" s="23"/>
       <c r="G362" s="24"/>
@@ -19713,10 +19724,10 @@
         <v>85</v>
       </c>
       <c r="D363" s="21" t="s">
+        <v>789</v>
+      </c>
+      <c r="E363" s="22" t="s">
         <v>790</v>
-      </c>
-      <c r="E363" s="22" t="s">
-        <v>791</v>
       </c>
       <c r="F363" s="23"/>
       <c r="G363" s="24"/>
@@ -19747,10 +19758,10 @@
         <v>85</v>
       </c>
       <c r="D364" s="21" t="s">
+        <v>791</v>
+      </c>
+      <c r="E364" s="22" t="s">
         <v>792</v>
-      </c>
-      <c r="E364" s="22" t="s">
-        <v>793</v>
       </c>
       <c r="F364" s="23"/>
       <c r="G364" s="24"/>
@@ -19781,10 +19792,10 @@
         <v>85</v>
       </c>
       <c r="D365" s="21" t="s">
+        <v>793</v>
+      </c>
+      <c r="E365" s="22" t="s">
         <v>794</v>
-      </c>
-      <c r="E365" s="22" t="s">
-        <v>795</v>
       </c>
       <c r="F365" s="23"/>
       <c r="G365" s="24"/>
@@ -19815,10 +19826,10 @@
         <v>85</v>
       </c>
       <c r="D366" s="21" t="s">
+        <v>795</v>
+      </c>
+      <c r="E366" s="22" t="s">
         <v>796</v>
-      </c>
-      <c r="E366" s="22" t="s">
-        <v>797</v>
       </c>
       <c r="F366" s="23"/>
       <c r="G366" s="24"/>
@@ -19849,10 +19860,10 @@
         <v>85</v>
       </c>
       <c r="D367" s="21" t="s">
+        <v>797</v>
+      </c>
+      <c r="E367" s="22" t="s">
         <v>798</v>
-      </c>
-      <c r="E367" s="22" t="s">
-        <v>799</v>
       </c>
       <c r="F367" s="23"/>
       <c r="G367" s="24"/>
@@ -19883,10 +19894,10 @@
         <v>85</v>
       </c>
       <c r="D368" s="21" t="s">
+        <v>799</v>
+      </c>
+      <c r="E368" s="22" t="s">
         <v>800</v>
-      </c>
-      <c r="E368" s="22" t="s">
-        <v>801</v>
       </c>
       <c r="F368" s="23"/>
       <c r="G368" s="24"/>
@@ -19917,10 +19928,10 @@
         <v>85</v>
       </c>
       <c r="D369" s="21" t="s">
+        <v>801</v>
+      </c>
+      <c r="E369" s="22" t="s">
         <v>802</v>
-      </c>
-      <c r="E369" s="22" t="s">
-        <v>803</v>
       </c>
       <c r="F369" s="23"/>
       <c r="G369" s="24"/>
@@ -19951,10 +19962,10 @@
         <v>85</v>
       </c>
       <c r="D370" s="21" t="s">
+        <v>803</v>
+      </c>
+      <c r="E370" s="22" t="s">
         <v>804</v>
-      </c>
-      <c r="E370" s="22" t="s">
-        <v>805</v>
       </c>
       <c r="F370" s="23"/>
       <c r="G370" s="24"/>
@@ -19985,10 +19996,10 @@
         <v>85</v>
       </c>
       <c r="D371" s="21" t="s">
+        <v>805</v>
+      </c>
+      <c r="E371" s="22" t="s">
         <v>806</v>
-      </c>
-      <c r="E371" s="22" t="s">
-        <v>807</v>
       </c>
       <c r="F371" s="23"/>
       <c r="G371" s="24"/>
@@ -20019,10 +20030,10 @@
         <v>85</v>
       </c>
       <c r="D372" s="21" t="s">
+        <v>807</v>
+      </c>
+      <c r="E372" s="22" t="s">
         <v>808</v>
-      </c>
-      <c r="E372" s="22" t="s">
-        <v>809</v>
       </c>
       <c r="F372" s="23"/>
       <c r="G372" s="24"/>
@@ -20053,10 +20064,10 @@
         <v>85</v>
       </c>
       <c r="D373" s="21" t="s">
+        <v>809</v>
+      </c>
+      <c r="E373" s="22" t="s">
         <v>810</v>
-      </c>
-      <c r="E373" s="22" t="s">
-        <v>811</v>
       </c>
       <c r="F373" s="23"/>
       <c r="G373" s="24"/>
@@ -20087,10 +20098,10 @@
         <v>49</v>
       </c>
       <c r="D374" s="21" t="s">
+        <v>811</v>
+      </c>
+      <c r="E374" s="22" t="s">
         <v>812</v>
-      </c>
-      <c r="E374" s="22" t="s">
-        <v>813</v>
       </c>
       <c r="F374" s="23"/>
       <c r="G374" s="24"/>
@@ -29737,7 +29748,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
@@ -29784,10 +29795,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>813</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>814</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1">
@@ -29795,13 +29806,13 @@
         <v>49</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>815</v>
+      </c>
+      <c r="C2" s="30" t="s">
         <v>816</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="D2" s="30" t="s">
         <v>817</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.25" customHeight="1">
@@ -29809,13 +29820,13 @@
         <v>56</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C3" s="30" t="s">
+        <v>818</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>819</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.25" customHeight="1">
@@ -29823,13 +29834,13 @@
         <v>61</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C4" s="30" t="s">
+        <v>820</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>821</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.25" customHeight="1">
@@ -29837,13 +29848,13 @@
         <v>66</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C5" s="30" t="s">
+        <v>822</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>823</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.25" customHeight="1">
@@ -29851,13 +29862,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C6" s="30" t="s">
+        <v>824</v>
+      </c>
+      <c r="D6" s="31" t="s">
         <v>825</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -29865,13 +29876,13 @@
         <v>76</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C7" s="30" t="s">
+        <v>826</v>
+      </c>
+      <c r="D7" s="31" t="s">
         <v>827</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -29879,13 +29890,13 @@
         <v>403</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C8" s="30" t="s">
+        <v>828</v>
+      </c>
+      <c r="D8" s="31" t="s">
         <v>829</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -29893,27 +29904,27 @@
         <v>85</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C9" s="30" t="s">
+        <v>830</v>
+      </c>
+      <c r="D9" s="31" t="s">
         <v>831</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.25" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C10" s="30">
         <v>191</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.25" customHeight="1">
@@ -29921,13 +29932,13 @@
         <v>49</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C11" s="30">
         <v>192</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.25" customHeight="1">
@@ -29935,13 +29946,13 @@
         <v>56</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C12" s="30">
         <v>208</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1">
@@ -29949,13 +29960,13 @@
         <v>61</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C13" s="30">
         <v>224</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1">
@@ -29963,13 +29974,13 @@
         <v>66</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C14" s="30">
         <v>240</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.25" customHeight="1">
@@ -29977,13 +29988,13 @@
         <v>71</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C15" s="30">
         <v>256</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.25" customHeight="1">
@@ -29991,13 +30002,13 @@
         <v>76</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C16" s="30">
         <v>272</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
@@ -30005,13 +30016,13 @@
         <v>403</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C17" s="30">
         <v>288</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.5" customHeight="1">
@@ -30019,13 +30030,13 @@
         <v>85</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C18" s="30">
         <v>304</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
@@ -30033,13 +30044,13 @@
         <v>49</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C19" s="30">
         <v>193</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1">
@@ -30047,13 +30058,13 @@
         <v>56</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C20" s="30">
         <v>209</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
@@ -30061,13 +30072,13 @@
         <v>61</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C21" s="30">
         <v>225</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
@@ -30075,13 +30086,13 @@
         <v>66</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C22" s="30">
         <v>241</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1">
@@ -30089,13 +30100,13 @@
         <v>71</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C23" s="30">
         <v>257</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
@@ -30103,13 +30114,13 @@
         <v>76</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C24" s="30">
         <v>273</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
@@ -30117,13 +30128,13 @@
         <v>403</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C25" s="30">
         <v>289</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1">
@@ -30131,13 +30142,13 @@
         <v>85</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C26" s="30">
         <v>305</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1">
@@ -30145,13 +30156,13 @@
         <v>49</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C27" s="30">
         <v>194</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1">
@@ -30159,13 +30170,13 @@
         <v>56</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C28" s="30">
         <v>210</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
@@ -30173,13 +30184,13 @@
         <v>61</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C29" s="30">
         <v>226</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1">
@@ -30187,13 +30198,13 @@
         <v>66</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C30" s="30">
         <v>242</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1">
@@ -30201,13 +30212,13 @@
         <v>71</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C31" s="30">
         <v>258</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1">
@@ -30215,13 +30226,13 @@
         <v>76</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C32" s="30">
         <v>274</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1">
@@ -30229,13 +30240,13 @@
         <v>403</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C33" s="30">
         <v>290</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1">
@@ -30243,13 +30254,13 @@
         <v>85</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C34" s="30">
         <v>306</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1">
@@ -30257,7 +30268,7 @@
         <v>49</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C35" s="30">
         <v>195</v>
@@ -30271,7 +30282,7 @@
         <v>56</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C36" s="30">
         <v>211</v>
@@ -30285,7 +30296,7 @@
         <v>61</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C37" s="30">
         <v>227</v>
@@ -30299,7 +30310,7 @@
         <v>66</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C38" s="30">
         <v>243</v>
@@ -30313,7 +30324,7 @@
         <v>71</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C39" s="30">
         <v>259</v>
@@ -30327,7 +30338,7 @@
         <v>76</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C40" s="30">
         <v>275</v>
@@ -30341,7 +30352,7 @@
         <v>403</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C41" s="30">
         <v>291</v>
@@ -30355,7 +30366,7 @@
         <v>85</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C42" s="30">
         <v>307</v>
@@ -30369,7 +30380,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C43" s="30">
         <v>196</v>
@@ -30383,7 +30394,7 @@
         <v>56</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C44" s="30">
         <v>212</v>
@@ -30397,7 +30408,7 @@
         <v>61</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C45" s="30">
         <v>228</v>
@@ -30411,7 +30422,7 @@
         <v>66</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C46" s="30">
         <v>244</v>
@@ -30425,7 +30436,7 @@
         <v>71</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C47" s="30">
         <v>260</v>
@@ -30439,7 +30450,7 @@
         <v>76</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C48" s="30">
         <v>276</v>
@@ -30453,7 +30464,7 @@
         <v>403</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C49" s="30">
         <v>292</v>
@@ -30467,7 +30478,7 @@
         <v>85</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C50" s="30">
         <v>308</v>
@@ -31452,7 +31463,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>215</v>
@@ -31460,7 +31471,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>218</v>
@@ -32477,6 +32488,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100794258E7DE47134588D45098EBDB60F8" ma:contentTypeVersion="6" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="3194f2ccada4dbd4f766fc5cce730de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0bdf65ce-24cf-486b-995b-57ece8b70f4e" xmlns:ns3="c50f76eb-a136-4a5c-b9b3-fbcc59ed104d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0b17b18953fe681e8c031b46ce8399c7" ns2:_="" ns3:_="">
     <xsd:import namespace="0bdf65ce-24cf-486b-995b-57ece8b70f4e"/>
@@ -32653,22 +32673,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C8BC82A-7102-4313-BB0C-4C51CC2434A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{097B1022-1E03-4022-B756-1D5D590C8ADC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32687,19 +32706,11 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67CBBC7B-62D8-4480-9D66-C095B0112D05}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C8BC82A-7102-4313-BB0C-4C51CC2434A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
correzioni per mancato accreditamento LDO ID6
commonName auth: "A1#111EXPRIVIA000"
subject_application_vendor: "exprivia"
subject_application_id: "aurora"
subject_application_version: "2"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/AURORA/2/report-checklist.xlsx
+++ b/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/AURORA/2/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exprivia.sharepoint.com/sites/DFEH-PS-FSE2.0adeguamenti/Documenti condivisi/Documenti Accreditamento/Accreditamento AURORA MERGE/2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03C6FE6E-4BC3-4516-B408-0A3BDCD8BB72}"/>
+  <xr:revisionPtr revIDLastSave="259" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AD70417-BEFC-4A1F-BF7B-A433DB27DCF8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="28800" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4104,15 +4104,6 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>2023-05-08T11:52:50Z</t>
-  </si>
-  <si>
-    <t>1f0a215946ee4092</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4.4.cc254550809f2948acda3f6d72cf35d0a2838c6f17f39b26126e2795a65d69c7.8273381a49^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-05-08T15:25:45Z</t>
   </si>
   <si>
@@ -4129,6 +4120,15 @@
   </si>
   <si>
     <t>2023-05-12T12:49:55Z</t>
+  </si>
+  <si>
+    <t>2023-05-16T14:43:00Z</t>
+  </si>
+  <si>
+    <t>d613073ed3750a52</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.4.4.2185d81dce95496029dd86f4e35350f4a2d0e6d9881c53d9677e51eed8774aae.b64e66b1fc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4497,7 +4497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4666,6 +4666,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7127,9 +7130,9 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="9" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="K207" sqref="K207"/>
+      <selection pane="bottomLeft" activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -10045,23 +10048,23 @@
       <c r="C88" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D88" s="21" t="s">
+      <c r="D88" s="61" t="s">
         <v>213</v>
       </c>
       <c r="E88" s="22" t="s">
         <v>214</v>
       </c>
       <c r="F88" s="23">
-        <v>45054</v>
+        <v>45062</v>
       </c>
       <c r="G88" s="24" t="s">
-        <v>865</v>
+        <v>871</v>
       </c>
       <c r="H88" s="24" t="s">
-        <v>866</v>
+        <v>872</v>
       </c>
       <c r="I88" s="24" t="s">
-        <v>867</v>
+        <v>873</v>
       </c>
       <c r="J88" s="25" t="s">
         <v>215</v>
@@ -14225,13 +14228,13 @@
         <v>45058</v>
       </c>
       <c r="G207" s="41" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="H207" s="41" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="I207" s="41" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="J207" s="33" t="s">
         <v>215</v>
@@ -14897,10 +14900,10 @@
         <v>45054</v>
       </c>
       <c r="G226" s="41" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="H226" s="41" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="I226" s="41" t="s">
         <v>297</v>
@@ -14916,7 +14919,7 @@
         <v>218</v>
       </c>
       <c r="N226" s="33" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="O226" s="33" t="s">
         <v>215</v>
@@ -32497,6 +32500,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100794258E7DE47134588D45098EBDB60F8" ma:contentTypeVersion="6" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="3194f2ccada4dbd4f766fc5cce730de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0bdf65ce-24cf-486b-995b-57ece8b70f4e" xmlns:ns3="c50f76eb-a136-4a5c-b9b3-fbcc59ed104d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0b17b18953fe681e8c031b46ce8399c7" ns2:_="" ns3:_="">
     <xsd:import namespace="0bdf65ce-24cf-486b-995b-57ece8b70f4e"/>
@@ -32673,12 +32682,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C8BC82A-7102-4313-BB0C-4C51CC2434A9}">
   <ds:schemaRefs>
@@ -32688,6 +32691,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67CBBC7B-62D8-4480-9D66-C095B0112D05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{097B1022-1E03-4022-B756-1D5D590C8ADC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32704,13 +32716,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67CBBC7B-62D8-4480-9D66-C095B0112D05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sostituito file checklist colonna n compilata
commonName auth: "A1#111EXPRIVIA000"
subject_application_vendor: "exprivia"
subject_application_id: "aurora"
subject_application_version: "2"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/AURORA/2/report-checklist.xlsx
+++ b/GATEWAY/A1#111EXPRIVIA000/EXPRIVIA/AURORA/2/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://exprivia.sharepoint.com/sites/DFEH-PS-FSE2.0adeguamenti/Documenti condivisi/Documenti Accreditamento/Accreditamento AURORA MERGE/2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="286" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15D4E2A4-4B4B-4746-A0BA-672A8EEF929D}"/>
+  <xr:revisionPtr revIDLastSave="288" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8689BA3-6C53-44AB-89A3-6A7616760F6A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="2925" windowWidth="28800" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -7159,10 +7159,10 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
-      <selection pane="bottomLeft" activeCell="L305" sqref="L305"/>
+      <selection pane="bottomLeft" activeCell="N125" sqref="N125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11356,7 +11356,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="20">
         <v>37</v>
       </c>
@@ -12856,7 +12856,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A167" s="20">
         <v>73</v>
       </c>
@@ -12908,7 +12908,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="330.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:20" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="20">
         <v>305</v>
       </c>
@@ -12942,7 +12942,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="20">
         <v>318</v>
       </c>
@@ -12976,7 +12976,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="170" spans="1:20" ht="255.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="20">
         <v>322</v>
       </c>
@@ -13010,7 +13010,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="171" spans="1:20" ht="285.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:20" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="20">
         <v>323</v>
       </c>
@@ -13044,7 +13044,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="20">
         <v>74</v>
       </c>
@@ -13082,7 +13082,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="315.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:20" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="20">
         <v>290</v>
       </c>
@@ -13116,7 +13116,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="270.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:20" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="20">
         <v>330</v>
       </c>
@@ -13150,7 +13150,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="20">
         <v>331</v>
       </c>
@@ -13184,7 +13184,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="255.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="20">
         <v>334</v>
       </c>
@@ -13218,7 +13218,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="177" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="20">
         <v>335</v>
       </c>
@@ -13252,7 +13252,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="178" spans="1:20" ht="270.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:20" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="20">
         <v>338</v>
       </c>
@@ -13286,7 +13286,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="179" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="20">
         <v>339</v>
       </c>
@@ -13320,7 +13320,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="270.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:20" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="20">
         <v>342</v>
       </c>
@@ -13354,7 +13354,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="300.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:20" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="20">
         <v>343</v>
       </c>
@@ -13388,7 +13388,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="270.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:20" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="20">
         <v>301</v>
       </c>
@@ -13422,7 +13422,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="225.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:20" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="20">
         <v>364</v>
       </c>
@@ -13456,7 +13456,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="255.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="20">
         <v>350</v>
       </c>
@@ -13490,7 +13490,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="285.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:20" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="20">
         <v>351</v>
       </c>
@@ -13524,7 +13524,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="20">
         <v>1</v>
       </c>
@@ -13558,7 +13558,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="20">
         <v>2</v>
       </c>
@@ -13592,7 +13592,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="20">
         <v>3</v>
       </c>
@@ -13626,7 +13626,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="20">
         <v>4</v>
       </c>
@@ -13660,7 +13660,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="20">
         <v>5</v>
       </c>
@@ -13694,7 +13694,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="173.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:20" ht="173.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A191" s="20">
         <v>365</v>
       </c>
@@ -13728,7 +13728,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="169.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:20" ht="169.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A192" s="20">
         <v>291</v>
       </c>
@@ -13762,7 +13762,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="169.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:20" ht="169.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A193" s="20">
         <v>300</v>
       </c>
@@ -13796,7 +13796,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="180.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:20" ht="180.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A194" s="20">
         <v>292</v>
       </c>
@@ -13830,7 +13830,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="20">
         <v>11</v>
       </c>
@@ -13864,7 +13864,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="20">
         <v>12</v>
       </c>
@@ -13898,7 +13898,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="20">
         <v>13</v>
       </c>
@@ -13932,7 +13932,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="20">
         <v>14</v>
       </c>
@@ -13966,7 +13966,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="20">
         <v>16</v>
       </c>
@@ -14000,7 +14000,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="20">
         <v>17</v>
       </c>
@@ -14034,7 +14034,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="20">
         <v>18</v>
       </c>
@@ -14068,7 +14068,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="20">
         <v>19</v>
       </c>
@@ -14102,7 +14102,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="203" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="20">
         <v>20</v>
       </c>
@@ -14136,7 +14136,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="20">
         <v>21</v>
       </c>
@@ -14170,7 +14170,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="20">
         <v>22</v>
       </c>
@@ -14204,7 +14204,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="20">
         <v>23</v>
       </c>
@@ -14238,7 +14238,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="37">
         <v>24</v>
       </c>
@@ -14282,7 +14282,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="37">
         <v>25</v>
       </c>
@@ -14320,7 +14320,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="209" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="37">
         <v>26</v>
       </c>
@@ -14358,7 +14358,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="210" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="37">
         <v>27</v>
       </c>
@@ -14396,7 +14396,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="1.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:20" ht="1.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A211" s="20">
         <v>28</v>
       </c>
@@ -14430,7 +14430,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="270.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:20" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="20">
         <v>303</v>
       </c>
@@ -14464,7 +14464,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="20">
         <v>30</v>
       </c>
@@ -14498,7 +14498,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="20">
         <v>31</v>
       </c>
@@ -14532,7 +14532,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="215" spans="1:20" ht="240.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="20">
         <v>288</v>
       </c>
@@ -14566,7 +14566,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="216" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="20">
         <v>33</v>
       </c>
@@ -14600,7 +14600,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="217" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="20">
         <v>34</v>
       </c>
@@ -14634,7 +14634,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="37">
         <v>35</v>
       </c>
@@ -14672,7 +14672,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="20">
         <v>36</v>
       </c>
@@ -14706,7 +14706,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="180.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:20" ht="180.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A220" s="20">
         <v>293</v>
       </c>
@@ -14740,7 +14740,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="221" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="20">
         <v>38</v>
       </c>
@@ -14774,7 +14774,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="20">
         <v>39</v>
       </c>
@@ -14808,7 +14808,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="223" spans="1:20" ht="255.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="20">
         <v>294</v>
       </c>
@@ -14842,7 +14842,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="224" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="20">
         <v>41</v>
       </c>
@@ -14876,7 +14876,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="225" spans="1:20" ht="180.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:20" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="20">
         <v>42</v>
       </c>
@@ -14910,7 +14910,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="47">
         <v>43</v>
       </c>
@@ -14964,7 +14964,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="20">
         <v>44</v>
       </c>
@@ -15000,7 +15000,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="228" spans="1:20" ht="60.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:20" ht="60.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A228" s="20">
         <v>295</v>
       </c>
@@ -15034,7 +15034,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="20">
         <v>46</v>
       </c>
@@ -15070,7 +15070,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="20">
         <v>47</v>
       </c>
@@ -15106,7 +15106,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="255.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:20" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="20">
         <v>296</v>
       </c>
@@ -15140,7 +15140,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="20">
         <v>49</v>
       </c>
@@ -15176,7 +15176,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="45.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:20" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="20">
         <v>50</v>
       </c>
@@ -15212,7 +15212,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="234" spans="1:20" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="20">
         <v>51</v>
       </c>
@@ -15260,7 +15260,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="235" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="20">
         <v>52</v>
       </c>
@@ -15294,7 +15294,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="20">
         <v>53</v>
       </c>
@@ -15328,7 +15328,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="20">
         <v>54</v>
       </c>
@@ -15362,7 +15362,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="20">
         <v>55</v>
       </c>
@@ -15396,7 +15396,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="20">
         <v>56</v>
       </c>
@@ -15430,7 +15430,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="20">
         <v>57</v>
       </c>
@@ -15464,7 +15464,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="20">
         <v>58</v>
       </c>
@@ -15498,7 +15498,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="20">
         <v>59</v>
       </c>
@@ -15532,7 +15532,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="243" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="20">
         <v>60</v>
       </c>
@@ -15566,7 +15566,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="244" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="20">
         <v>61</v>
       </c>
@@ -15600,7 +15600,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="20">
         <v>62</v>
       </c>
@@ -15634,7 +15634,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="246" spans="1:20" ht="139.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:20" ht="139.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A246" s="20">
         <v>297</v>
       </c>
@@ -15668,7 +15668,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="247" spans="1:20" ht="149.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:20" ht="149.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A247" s="20">
         <v>298</v>
       </c>
@@ -15702,7 +15702,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="248" spans="1:20" ht="143.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:20" ht="143.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A248" s="20">
         <v>299</v>
       </c>
@@ -15736,7 +15736,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="249" spans="1:20" ht="149.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:20" ht="149.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A249" s="20">
         <v>344</v>
       </c>
@@ -15770,7 +15770,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="250" spans="1:20" ht="131.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:20" ht="131.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A250" s="20">
         <v>345</v>
       </c>
@@ -15804,7 +15804,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="251" spans="1:20" ht="129" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:20" ht="129" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A251" s="20">
         <v>289</v>
       </c>
@@ -15838,7 +15838,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="252" spans="1:20" ht="132.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:20" ht="132.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A252" s="20">
         <v>302</v>
       </c>
@@ -15872,7 +15872,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="253" spans="1:20" ht="130.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:20" ht="130.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A253" s="20">
         <v>346</v>
       </c>
@@ -15906,7 +15906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="126.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:20" ht="126.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A254" s="20">
         <v>347</v>
       </c>
@@ -15940,7 +15940,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="130.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:20" ht="130.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A255" s="20">
         <v>32</v>
       </c>
@@ -15974,7 +15974,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="128.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:20" ht="128.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A256" s="20">
         <v>40</v>
       </c>
@@ -16008,7 +16008,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="124.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:20" ht="124.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A257" s="20">
         <v>48</v>
       </c>
@@ -16044,7 +16044,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="20">
         <v>75</v>
       </c>
@@ -16078,7 +16078,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="20">
         <v>76</v>
       </c>
@@ -16112,7 +16112,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="20">
         <v>77</v>
       </c>
@@ -16146,7 +16146,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="20">
         <v>78</v>
       </c>
@@ -16180,7 +16180,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="20">
         <v>79</v>
       </c>
@@ -16214,7 +16214,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="263" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="20">
         <v>80</v>
       </c>
@@ -16248,7 +16248,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="20">
         <v>81</v>
       </c>
@@ -16282,7 +16282,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="265" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="20">
         <v>82</v>
       </c>
@@ -16316,7 +16316,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="266" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="20">
         <v>83</v>
       </c>
@@ -16350,7 +16350,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="267" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="20">
         <v>84</v>
       </c>
@@ -16384,7 +16384,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="268" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="20">
         <v>85</v>
       </c>
@@ -16418,7 +16418,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="269" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="20">
         <v>86</v>
       </c>
@@ -16452,7 +16452,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="20">
         <v>87</v>
       </c>
@@ -16486,7 +16486,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="271" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="20">
         <v>88</v>
       </c>
@@ -16520,7 +16520,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="272" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="20">
         <v>89</v>
       </c>
@@ -16554,7 +16554,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="273" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="20">
         <v>90</v>
       </c>
@@ -16588,7 +16588,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="274" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="20">
         <v>91</v>
       </c>
@@ -16622,7 +16622,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="275" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="20">
         <v>92</v>
       </c>
@@ -16656,7 +16656,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="276" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="20">
         <v>93</v>
       </c>
@@ -16690,7 +16690,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="20">
         <v>94</v>
       </c>
@@ -16724,7 +16724,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="20">
         <v>95</v>
       </c>
@@ -16758,7 +16758,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="20">
         <v>96</v>
       </c>
@@ -16792,7 +16792,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="20">
         <v>97</v>
       </c>
@@ -16826,7 +16826,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="281" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="20">
         <v>98</v>
       </c>
@@ -16860,7 +16860,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="282" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="20">
         <v>99</v>
       </c>
@@ -16894,7 +16894,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="283" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="20">
         <v>100</v>
       </c>
@@ -16928,7 +16928,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="284" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="20">
         <v>101</v>
       </c>
@@ -16962,7 +16962,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="20">
         <v>102</v>
       </c>
@@ -16996,7 +16996,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="20">
         <v>103</v>
       </c>
@@ -17030,7 +17030,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="20">
         <v>104</v>
       </c>
@@ -17064,7 +17064,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="20">
         <v>105</v>
       </c>
@@ -17098,7 +17098,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:20" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="20">
         <v>106</v>
       </c>
@@ -17132,7 +17132,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="290" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="20">
         <v>107</v>
       </c>
@@ -17166,7 +17166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="291" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="20">
         <v>108</v>
       </c>
@@ -17200,7 +17200,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="292" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="20">
         <v>109</v>
       </c>
@@ -17234,7 +17234,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="293" spans="1:20" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="20">
         <v>110</v>
       </c>
@@ -17268,7 +17268,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="20">
         <v>111</v>
       </c>
@@ -17302,7 +17302,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="295" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="20">
         <v>112</v>
       </c>
@@ -17336,7 +17336,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="296" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="20">
         <v>113</v>
       </c>
@@ -17370,7 +17370,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="297" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="20">
         <v>114</v>
       </c>
@@ -17404,7 +17404,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="298" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="20">
         <v>115</v>
       </c>
@@ -17438,7 +17438,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="20">
         <v>116</v>
       </c>
@@ -17472,7 +17472,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="300" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="20">
         <v>117</v>
       </c>
@@ -17506,7 +17506,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="301" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="20">
         <v>118</v>
       </c>
@@ -17540,7 +17540,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="20">
         <v>119</v>
       </c>
@@ -17574,7 +17574,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="303" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="20">
         <v>120</v>
       </c>
@@ -17608,7 +17608,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="20">
         <v>121</v>
       </c>
@@ -17642,7 +17642,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="305" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="20">
         <v>122</v>
       </c>
@@ -17680,7 +17680,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="306" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="20">
         <v>123</v>
       </c>
@@ -17718,7 +17718,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="20">
         <v>124</v>
       </c>
@@ -17756,7 +17756,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="20">
         <v>125</v>
       </c>
@@ -17794,7 +17794,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="20">
         <v>126</v>
       </c>
@@ -17832,7 +17832,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="20">
         <v>127</v>
       </c>
@@ -17870,7 +17870,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="20">
         <v>128</v>
       </c>
@@ -17908,7 +17908,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="20">
         <v>129</v>
       </c>
@@ -17946,7 +17946,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="20">
         <v>130</v>
       </c>
@@ -17984,7 +17984,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="314" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="20">
         <v>131</v>
       </c>
@@ -18022,7 +18022,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="315" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="20">
         <v>132</v>
       </c>
@@ -18060,7 +18060,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="316" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="20">
         <v>133</v>
       </c>
@@ -18098,7 +18098,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="20">
         <v>134</v>
       </c>
@@ -18136,7 +18136,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="318" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="20">
         <v>135</v>
       </c>
@@ -18174,7 +18174,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="20">
         <v>136</v>
       </c>
@@ -18212,7 +18212,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="20">
         <v>137</v>
       </c>
@@ -18250,7 +18250,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="20">
         <v>138</v>
       </c>
@@ -18288,7 +18288,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="20">
         <v>139</v>
       </c>
@@ -18326,7 +18326,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="323" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="20">
         <v>140</v>
       </c>
@@ -18364,7 +18364,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="324" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="20">
         <v>141</v>
       </c>
@@ -18402,7 +18402,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="325" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:20" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="20">
         <v>142</v>
       </c>
@@ -18456,7 +18456,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="326" spans="1:20" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:20" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="20">
         <v>143</v>
       </c>
@@ -18510,7 +18510,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="327" spans="1:20" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:20" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="20">
         <v>144</v>
       </c>
@@ -18548,7 +18548,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="328" spans="1:20" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="20">
         <v>145</v>
       </c>
@@ -18586,7 +18586,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="329" spans="1:20" ht="150" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:20" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="20">
         <v>146</v>
       </c>
@@ -29752,6 +29752,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T374" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="37"/>
+        <filter val="73"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="1">
       <filters>
         <filter val="VALIDAZIONE"/>
@@ -29759,6 +29765,7 @@
     </filterColumn>
     <filterColumn colId="2">
       <filters>
+        <filter val="LDO"/>
         <filter val="VPS"/>
       </filters>
     </filterColumn>
@@ -32520,21 +32527,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100794258E7DE47134588D45098EBDB60F8" ma:contentTypeVersion="6" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="3194f2ccada4dbd4f766fc5cce730de0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0bdf65ce-24cf-486b-995b-57ece8b70f4e" xmlns:ns3="c50f76eb-a136-4a5c-b9b3-fbcc59ed104d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0b17b18953fe681e8c031b46ce8399c7" ns2:_="" ns3:_="">
     <xsd:import namespace="0bdf65ce-24cf-486b-995b-57ece8b70f4e"/>
@@ -32711,24 +32703,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67CBBC7B-62D8-4480-9D66-C095B0112D05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C8BC82A-7102-4313-BB0C-4C51CC2434A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{097B1022-1E03-4022-B756-1D5D590C8ADC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -32745,4 +32735,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C8BC82A-7102-4313-BB0C-4C51CC2434A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67CBBC7B-62D8-4480-9D66-C095B0112D05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>